<commit_message>
made yml file specific to windows because of issues. some other trivial things.
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\data\sodankyla_cam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8427F16E-2926-4565-9FAD-CF50FC4221CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C8C481-7CDB-4525-A9AE-101F2FAB8D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{D49610C9-570A-4CC9-A688-ECF1C599658C}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="1" xr2:uid="{D49610C9-570A-4CC9-A688-ECF1C599658C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="125">
   <si>
     <t>Lompolojänkkä Peatland</t>
   </si>
@@ -1560,8 +1560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E651408-387C-4106-A9DC-EC26E0A848EE}">
   <dimension ref="A1:F206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2058,154 +2058,116 @@
       <c r="A25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>43501</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>43551</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <v>43592</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1">
+        <v>43773</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43864</v>
+      </c>
+    </row>
     <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="46" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="49" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="50" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="51" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="52" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="53" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="54" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="55" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="56" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="58" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="59" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="60" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="63" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="65" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="66" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="67" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed parallel.py issues regarding atl03 files getting appended incorrectly before plotting because some files are technically not empty even though the section we are cropping to is; processed files were already getting skipped but the same thing pulled from the full file was not. Have successfully replicated the processed data from the full data (give or take some data points because of the whole 1 degree = 111-113 kilometers thing instead of the assumed 100, effect is bigger the larger the region of interest is), now need to go back and classify more images for FSC because the number of tracks around the Sodankyla cam has doubled from 35 to 70 because we are keeping all the tracks that went missing during preprocessing in DAAC.
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C8C481-7CDB-4525-A9AE-101F2FAB8D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC315201-3813-4721-9A73-9B85B098BB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="1" xr2:uid="{D49610C9-570A-4CC9-A688-ECF1C599658C}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="19140" windowHeight="11400" activeTab="1" xr2:uid="{D49610C9-570A-4CC9-A688-ECF1C599658C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1560,7 +1560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E651408-387C-4106-A9DC-EC26E0A848EE}">
   <dimension ref="A1:F206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modified the snow cam detail sheet to get rid of file number since I don't want to rely on it and to fit the new naming convention that relies on file name
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC315201-3813-4721-9A73-9B85B098BB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1674240-F43A-4857-A428-B255DA9FD58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="19140" windowHeight="11400" activeTab="1" xr2:uid="{D49610C9-570A-4CC9-A688-ECF1C599658C}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="1" xr2:uid="{D49610C9-570A-4CC9-A688-ECF1C599658C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="125">
   <si>
     <t>Lompolojänkkä Peatland</t>
   </si>
@@ -325,15 +325,9 @@
     <t>Usable File Numbers</t>
   </si>
   <si>
-    <t>File Number</t>
-  </si>
-  <si>
     <t>FSC</t>
   </si>
   <si>
-    <t>Sodankyla Intensive Observation Area</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -410,6 +404,12 @@
   </si>
   <si>
     <t>Tree Snow</t>
+  </si>
+  <si>
+    <t>sodankyla_full</t>
+  </si>
+  <si>
+    <t>kenttarova_full</t>
   </si>
 </sst>
 </file>
@@ -1558,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E651408-387C-4106-A9DC-EC26E0A848EE}">
-  <dimension ref="A1:F206"/>
+  <dimension ref="A1:E206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1569,573 +1569,481 @@
     <col min="1" max="1" width="39.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.26953125" customWidth="1"/>
     <col min="3" max="3" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="42.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7265625" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
         <v>96</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43477</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43489</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43551</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43568</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43580</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43630</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43841</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43932</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43993</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44084</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44306</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44357</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44386</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44447</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44459</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44550</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44579</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44670</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44720</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44992</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45004</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45021</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45124</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>124</v>
       </c>
-      <c r="F1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>43477</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43489</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B25" s="1">
+        <v>43501</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="1">
         <v>43551</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43568</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>43580</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>43630</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1">
-        <v>43841</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1">
-        <v>43932</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1">
-        <v>43993</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44084</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1">
-        <v>44306</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1">
-        <v>44357</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1">
-        <v>44386</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1">
-        <v>44447</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1">
-        <v>44459</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17">
-        <v>23</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44550</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1">
-        <v>44579</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1">
-        <v>44670</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20">
-        <v>26</v>
-      </c>
-      <c r="C20" s="1">
-        <v>44720</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21">
-        <v>30</v>
-      </c>
-      <c r="C21" s="1">
-        <v>44992</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22">
-        <v>31</v>
-      </c>
-      <c r="C22" s="1">
-        <v>45004</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23">
-        <v>32</v>
-      </c>
-      <c r="C23" s="1">
-        <v>45021</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24">
-        <v>35</v>
-      </c>
-      <c r="C24" s="1">
-        <v>45124</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>43501</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1">
-        <v>43551</v>
+      <c r="C26">
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1">
+        <v>124</v>
+      </c>
+      <c r="B27" s="1">
         <v>43592</v>
       </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
       <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28">
-        <v>4</v>
-      </c>
-      <c r="C28" s="1">
+        <v>124</v>
+      </c>
+      <c r="B28" s="1">
         <v>43773</v>
       </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1">
-        <v>43864</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    </row>
+    <row r="29" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="33" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="34" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="35" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2312,29 +2220,29 @@
     <row r="206" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190112_133002_Ccam1.jpg" xr:uid="{F7E00D50-9B4E-445D-9D07-1D001CF8D6AB}"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190124_124501_Ccam1.jpg" xr:uid="{129F43C4-EF41-4796-86C0-516EBA5E5912}"/>
-    <hyperlink ref="F4" r:id="rId3" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190327_123004_Ccam1.jpg" xr:uid="{E3C6F25E-BC26-400C-818B-725E1A9E89E3}"/>
-    <hyperlink ref="F5" r:id="rId4" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190413_143002_Ccam1.jpg" xr:uid="{BEBB4706-6A78-4BA6-BBAE-A66C746A84DA}"/>
-    <hyperlink ref="F6" r:id="rId5" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190425_073002_Ccam1.jpg" xr:uid="{7379D225-FCFC-406F-A107-FCD916D4FFCE}"/>
-    <hyperlink ref="F7" r:id="rId6" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190614_120002_Ccam1.jpg" xr:uid="{93EFA539-4049-4039-94E8-DCFA6F903A50}"/>
-    <hyperlink ref="F8" r:id="rId7" display="https://litdb.fmi.fi/data/webcam/Ccam1/2020/200111_100002_Ccam1.jpg" xr:uid="{173E0F8F-045C-46AC-A714-A89708AFE111}"/>
-    <hyperlink ref="F9" r:id="rId8" display="https://litdb.fmi.fi/data/webcam/Ccam1/2020/200411_160002_Ccam1.jpg" xr:uid="{52914D73-426F-4D48-AC69-A7FF3703497B}"/>
-    <hyperlink ref="F10" r:id="rId9" display="https://litdb.fmi.fi/data/webcam/Ccam1/2020/200611_131502_Ccam1.jpg" xr:uid="{52E08B2A-96B0-44B1-9C2E-C6F6CF1961C0}"/>
-    <hyperlink ref="F11" r:id="rId10" display="https://litdb.fmi.fi/data/webcam/Ccam1/2020/200910_164501_Ccam1.jpg" xr:uid="{41C3E6A6-2BCA-49D1-AF31-21F2B6CAE80A}"/>
-    <hyperlink ref="F12" r:id="rId11" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/210420_070002_Ccam1.jpg" xr:uid="{40108110-95B0-4503-B8A0-F0592F9BB2AF}"/>
-    <hyperlink ref="F13" r:id="rId12" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/210610_150002_Ccam1.jpg" xr:uid="{A2E424E6-892B-4BE6-8BAF-4819B7030EE4}"/>
-    <hyperlink ref="F14" r:id="rId13" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/210709_151502_Ccam1.jpg" xr:uid="{27620E8D-1F24-4D0C-8D97-703E8135CB87}"/>
-    <hyperlink ref="F15" r:id="rId14" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/210908_151502_Ccam1.jpg" xr:uid="{B95E404D-BD0A-4178-AB45-E2C9402CD218}"/>
-    <hyperlink ref="F16" r:id="rId15" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/210920_101502_Ccam1.jpg" xr:uid="{AD01C596-ABA8-453C-BE09-E104768F661D}"/>
-    <hyperlink ref="F17" r:id="rId16" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/211220_140002_Ccam1.jpg" xr:uid="{6E04B2BE-062A-4A04-839C-D6416798150D}"/>
-    <hyperlink ref="F18" r:id="rId17" display="https://litdb.fmi.fi/data/webcam/Ccam1/2022/220118_121502_Ccam1.jpg" xr:uid="{92717F46-E58B-45FC-BD7C-42BC0D96FCA6}"/>
-    <hyperlink ref="F19" r:id="rId18" display="https://litdb.fmi.fi/data/webcam/Ccam1/2022/220419_130002_Ccam1.jpg" xr:uid="{C50DC52D-2A31-47C8-9F69-D454C1C1350E}"/>
-    <hyperlink ref="F21" r:id="rId19" display="https://litdb.fmi.fi/data/webcam/Ccam1/2023/230307_100002_Ccam1.jpg" xr:uid="{95B9BE43-8D32-40A9-BBA0-179AD643BB55}"/>
-    <hyperlink ref="F22" r:id="rId20" display="https://litdb.fmi.fi/data/webcam/Ccam1/2023/230319_144502_Ccam1.jpg" xr:uid="{9AB7DB83-DE78-455B-89BD-9569AD45F3A0}"/>
-    <hyperlink ref="F20" r:id="rId21" display="https://litdb.fmi.fi/data/webcam/Ccam1/2022/220608_161501_Ccam1.jpg" xr:uid="{E559286A-AFA2-4375-AD71-0F7A128BD6B9}"/>
-    <hyperlink ref="F23" r:id="rId22" display="https://litdb.fmi.fi/data/webcam/Ccam1/2023/230405_140002_Ccam1.jpg" xr:uid="{212D602B-24E3-4D9D-B883-3D77A4D04881}"/>
-    <hyperlink ref="F24" r:id="rId23" display="https://litdb.fmi.fi/data/webcam/Ccam1/2023/230717_110002_Ccam1.jpg" xr:uid="{DCD013AD-D4F2-4ED9-880C-2EDB79F5C5D4}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190112_133002_Ccam1.jpg" xr:uid="{F7E00D50-9B4E-445D-9D07-1D001CF8D6AB}"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190124_124501_Ccam1.jpg" xr:uid="{129F43C4-EF41-4796-86C0-516EBA5E5912}"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190327_123004_Ccam1.jpg" xr:uid="{E3C6F25E-BC26-400C-818B-725E1A9E89E3}"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190413_143002_Ccam1.jpg" xr:uid="{BEBB4706-6A78-4BA6-BBAE-A66C746A84DA}"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190425_073002_Ccam1.jpg" xr:uid="{7379D225-FCFC-406F-A107-FCD916D4FFCE}"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://litdb.fmi.fi/data/webcam/Ccam1/2019/190614_120002_Ccam1.jpg" xr:uid="{93EFA539-4049-4039-94E8-DCFA6F903A50}"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://litdb.fmi.fi/data/webcam/Ccam1/2020/200111_100002_Ccam1.jpg" xr:uid="{173E0F8F-045C-46AC-A714-A89708AFE111}"/>
+    <hyperlink ref="E9" r:id="rId8" display="https://litdb.fmi.fi/data/webcam/Ccam1/2020/200411_160002_Ccam1.jpg" xr:uid="{52914D73-426F-4D48-AC69-A7FF3703497B}"/>
+    <hyperlink ref="E10" r:id="rId9" display="https://litdb.fmi.fi/data/webcam/Ccam1/2020/200611_131502_Ccam1.jpg" xr:uid="{52E08B2A-96B0-44B1-9C2E-C6F6CF1961C0}"/>
+    <hyperlink ref="E11" r:id="rId10" display="https://litdb.fmi.fi/data/webcam/Ccam1/2020/200910_164501_Ccam1.jpg" xr:uid="{41C3E6A6-2BCA-49D1-AF31-21F2B6CAE80A}"/>
+    <hyperlink ref="E12" r:id="rId11" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/210420_070002_Ccam1.jpg" xr:uid="{40108110-95B0-4503-B8A0-F0592F9BB2AF}"/>
+    <hyperlink ref="E13" r:id="rId12" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/210610_150002_Ccam1.jpg" xr:uid="{A2E424E6-892B-4BE6-8BAF-4819B7030EE4}"/>
+    <hyperlink ref="E14" r:id="rId13" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/210709_151502_Ccam1.jpg" xr:uid="{27620E8D-1F24-4D0C-8D97-703E8135CB87}"/>
+    <hyperlink ref="E15" r:id="rId14" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/210908_151502_Ccam1.jpg" xr:uid="{B95E404D-BD0A-4178-AB45-E2C9402CD218}"/>
+    <hyperlink ref="E16" r:id="rId15" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/210920_101502_Ccam1.jpg" xr:uid="{AD01C596-ABA8-453C-BE09-E104768F661D}"/>
+    <hyperlink ref="E17" r:id="rId16" display="https://litdb.fmi.fi/data/webcam/Ccam1/2021/211220_140002_Ccam1.jpg" xr:uid="{6E04B2BE-062A-4A04-839C-D6416798150D}"/>
+    <hyperlink ref="E18" r:id="rId17" display="https://litdb.fmi.fi/data/webcam/Ccam1/2022/220118_121502_Ccam1.jpg" xr:uid="{92717F46-E58B-45FC-BD7C-42BC0D96FCA6}"/>
+    <hyperlink ref="E19" r:id="rId18" display="https://litdb.fmi.fi/data/webcam/Ccam1/2022/220419_130002_Ccam1.jpg" xr:uid="{C50DC52D-2A31-47C8-9F69-D454C1C1350E}"/>
+    <hyperlink ref="E21" r:id="rId19" display="https://litdb.fmi.fi/data/webcam/Ccam1/2023/230307_100002_Ccam1.jpg" xr:uid="{95B9BE43-8D32-40A9-BBA0-179AD643BB55}"/>
+    <hyperlink ref="E22" r:id="rId20" display="https://litdb.fmi.fi/data/webcam/Ccam1/2023/230319_144502_Ccam1.jpg" xr:uid="{9AB7DB83-DE78-455B-89BD-9569AD45F3A0}"/>
+    <hyperlink ref="E20" r:id="rId21" display="https://litdb.fmi.fi/data/webcam/Ccam1/2022/220608_161501_Ccam1.jpg" xr:uid="{E559286A-AFA2-4375-AD71-0F7A128BD6B9}"/>
+    <hyperlink ref="E23" r:id="rId22" display="https://litdb.fmi.fi/data/webcam/Ccam1/2023/230405_140002_Ccam1.jpg" xr:uid="{212D602B-24E3-4D9D-B883-3D77A4D04881}"/>
+    <hyperlink ref="E24" r:id="rId23" display="https://litdb.fmi.fi/data/webcam/Ccam1/2023/230717_110002_Ccam1.jpg" xr:uid="{DCD013AD-D4F2-4ED9-880C-2EDB79F5C5D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>

</xml_diff>

<commit_message>
FSC_dataframe construction is closer to its form, but now it is completely jamming up in the computation of the coefficients. Not sure why. Need to look later.
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1674240-F43A-4857-A428-B255DA9FD58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF75EA29-7839-4A63-9CC7-562FE34F63F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="1" xr2:uid="{D49610C9-570A-4CC9-A688-ECF1C599658C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{D49610C9-570A-4CC9-A688-ECF1C599658C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="128">
   <si>
     <t>Lompolojänkkä Peatland</t>
   </si>
@@ -410,6 +410,15 @@
   </si>
   <si>
     <t>kenttarova_full</t>
+  </si>
+  <si>
+    <t>Coords</t>
+  </si>
+  <si>
+    <t>(26.634154, 67.361833)</t>
+  </si>
+  <si>
+    <t>(24.242983, 67.987283)</t>
   </si>
 </sst>
 </file>
@@ -1558,23 +1567,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E651408-387C-4106-A9DC-EC26E0A848EE}">
-  <dimension ref="A1:E206"/>
+  <dimension ref="A1:F206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.08984375" customWidth="1"/>
     <col min="2" max="2" width="14.26953125" customWidth="1"/>
     <col min="3" max="3" width="13.26953125" customWidth="1"/>
     <col min="5" max="5" width="42.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1590,8 +1599,11 @@
       <c r="E1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -1607,8 +1619,11 @@
       <c r="E2" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -1624,8 +1639,11 @@
       <c r="E3" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -1641,8 +1659,11 @@
       <c r="E4" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -1658,8 +1679,11 @@
       <c r="E5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -1675,8 +1699,11 @@
       <c r="E6" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -1692,8 +1719,11 @@
       <c r="E7" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -1709,8 +1739,11 @@
       <c r="E8" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -1726,8 +1759,11 @@
       <c r="E9" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -1743,8 +1779,11 @@
       <c r="E10" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -1760,8 +1799,11 @@
       <c r="E11" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -1777,8 +1819,11 @@
       <c r="E12" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>123</v>
       </c>
@@ -1794,8 +1839,11 @@
       <c r="E13" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -1811,8 +1859,11 @@
       <c r="E14" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>123</v>
       </c>
@@ -1828,8 +1879,11 @@
       <c r="E15" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -1845,8 +1899,11 @@
       <c r="E16" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -1862,8 +1919,11 @@
       <c r="E17" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -1879,8 +1939,11 @@
       <c r="E18" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -1896,8 +1959,11 @@
       <c r="E19" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -1913,8 +1979,11 @@
       <c r="E20" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -1930,8 +1999,11 @@
       <c r="E21" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>123</v>
       </c>
@@ -1947,8 +2019,11 @@
       <c r="E22" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>123</v>
       </c>
@@ -1964,8 +2039,11 @@
       <c r="E23" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -1981,8 +2059,11 @@
       <c r="E24" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -1995,8 +2076,11 @@
       <c r="D25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -2009,8 +2093,11 @@
       <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>124</v>
       </c>
@@ -2023,8 +2110,11 @@
       <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -2037,13 +2127,16 @@
       <c r="D28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="33" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="34" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="35" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
testing still, moving to filtering soonish
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -834,19 +834,19 @@
   </sheetPr>
   <dimension ref="A1:K307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C86" activeCellId="0" sqref="C86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="8.89"/>
   </cols>
@@ -2535,7 +2535,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
layer_flag seems to be a pretty good filtering tool in delta junction so far. want to look at other sites too. promising
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -834,17 +834,17 @@
   </sheetPr>
   <dimension ref="A1:K307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E81" activeCellId="0" sqref="E81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.44"/>
@@ -3010,6 +3010,12 @@
       </c>
       <c r="B81" s="3" t="n">
         <v>45317.2014930556</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="0" t="n">

</xml_diff>

<commit_message>
got rid of superfluous (and faulty) datasets. updated snow_cam_details.
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -605,9 +605,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -724,7 +725,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -742,6 +743,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -834,11 +839,11 @@
   </sheetPr>
   <dimension ref="A1:K307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E81" activeCellId="0" sqref="E81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
@@ -882,7 +887,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>43477.9055439815</v>
+        <v>43477</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
@@ -902,14 +907,15 @@
       <c r="H2" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>43489.3571064815</v>
+        <v>43489</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
@@ -929,14 +935,15 @@
       <c r="H3" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>43551.2347222222</v>
+        <v>43551</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -956,14 +963,15 @@
       <c r="H4" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>43568.7249305556</v>
+        <v>43568</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1</v>
@@ -983,19 +991,20 @@
       <c r="H5" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>43580.1763888889</v>
+        <v>43580</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0.9</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1010,14 +1019,15 @@
       <c r="H6" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>43630.6024421296</v>
+        <v>43630</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0</v>
@@ -1037,14 +1047,15 @@
       <c r="H7" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>43642.053900463</v>
+        <v>43642</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0</v>
@@ -1064,14 +1075,15 @@
       <c r="H8" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>43761.815</v>
+        <v>43761</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0.9</v>
@@ -1091,14 +1103,15 @@
       <c r="H9" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>43841.1827662037</v>
+        <v>43841</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>1</v>
@@ -1118,14 +1131,15 @@
       <c r="H10" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>43852.6342476852</v>
+        <v>43852</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>1</v>
@@ -1145,14 +1159,15 @@
       <c r="H11" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>43914.5118171296</v>
+        <v>43914</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>1</v>
@@ -1172,14 +1187,15 @@
       <c r="H12" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3" t="n">
-        <v>43932.0020601852</v>
+        <v>43932</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1</v>
@@ -1199,14 +1215,15 @@
       <c r="H13" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>43943.4535648148</v>
+        <v>43943</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>1</v>
@@ -1226,14 +1243,15 @@
       <c r="H14" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="3" t="n">
-        <v>43993.8796527778</v>
+        <v>43993</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -1253,14 +1271,15 @@
       <c r="H15" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>44005.3311458333</v>
+        <v>44005</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -1280,16 +1299,17 @@
       <c r="H16" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="3" t="n">
-        <v>44022.8213425926</v>
-      </c>
-      <c r="C17" s="6" t="n">
+        <v>44022</v>
+      </c>
+      <c r="C17" s="7" t="n">
         <v>0</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -1307,16 +1327,17 @@
       <c r="H17" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="3" t="n">
-        <v>44084.6989699074</v>
-      </c>
-      <c r="C18" s="6" t="n">
+        <v>44084</v>
+      </c>
+      <c r="C18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="0" t="n">
@@ -1334,16 +1355,17 @@
       <c r="H18" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="K18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="3" t="n">
-        <v>44125.0921296296</v>
-      </c>
-      <c r="C19" s="6" t="n">
+        <v>44125</v>
+      </c>
+      <c r="C19" s="7" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -1361,16 +1383,17 @@
       <c r="H19" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="K19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="3" t="n">
-        <v>44295.279375</v>
-      </c>
-      <c r="C20" s="6" t="n">
+        <v>44295</v>
+      </c>
+      <c r="C20" s="7" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="0" t="n">
@@ -1388,16 +1411,17 @@
       <c r="H20" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="K20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="3" t="n">
-        <v>44306.7308680556</v>
-      </c>
-      <c r="C21" s="6" t="n">
+        <v>44306</v>
+      </c>
+      <c r="C21" s="7" t="n">
         <v>0.9</v>
       </c>
       <c r="D21" s="0" t="n">
@@ -1415,14 +1439,15 @@
       <c r="H21" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="3" t="n">
-        <v>44357.1570138889</v>
+        <v>44357</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
@@ -1442,14 +1467,15 @@
       <c r="H22" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="K22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="3" t="n">
-        <v>44386.0987037037</v>
+        <v>44386</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>0</v>
@@ -1469,14 +1495,15 @@
       <c r="H23" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="3" t="n">
-        <v>44397.5501967593</v>
+        <v>44397</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>0</v>
@@ -1496,14 +1523,15 @@
       <c r="H24" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="K24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="3" t="n">
-        <v>44447.976400463</v>
+        <v>44447</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>0</v>
@@ -1523,14 +1551,15 @@
       <c r="H25" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="K25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="3" t="n">
-        <v>44459.4278819444</v>
+        <v>44459</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>0</v>
@@ -1550,14 +1579,15 @@
       <c r="H26" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="K26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="3" t="n">
-        <v>44476.9181365741</v>
+        <v>44476</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>0</v>
@@ -1577,14 +1607,15 @@
       <c r="H27" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="3" t="n">
-        <v>44550.2472800926</v>
+        <v>44550</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>1</v>
@@ -1604,14 +1635,15 @@
       <c r="H28" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="K28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="3" t="n">
-        <v>44579.1889930556</v>
+        <v>44579</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>1</v>
@@ -1631,14 +1663,15 @@
       <c r="H29" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="3" t="n">
-        <v>44670.0082638889</v>
+        <v>44670</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>1</v>
@@ -1658,14 +1691,15 @@
       <c r="H30" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="K30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="3" t="n">
-        <v>44720.4345023148</v>
+        <v>44720</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>0</v>
@@ -1685,14 +1719,15 @@
       <c r="H31" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="K31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="3" t="n">
-        <v>44749.3762731482</v>
+        <v>44749</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>0</v>
@@ -1712,14 +1747,15 @@
       <c r="H32" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="K32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="3" t="n">
-        <v>44760.8277430556</v>
+        <v>44760</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>0</v>
@@ -1739,14 +1775,15 @@
       <c r="H33" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="K33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="3" t="n">
-        <v>44851.6470717593</v>
+        <v>44851</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>0</v>
@@ -1766,14 +1803,15 @@
       <c r="H34" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="K34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="3" t="n">
-        <v>44992.8924768519</v>
+        <v>44992</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>1</v>
@@ -1793,14 +1831,15 @@
       <c r="H35" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="K35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="3" t="n">
-        <v>45004.3440393519</v>
+        <v>45004</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>1</v>
@@ -1820,14 +1859,15 @@
       <c r="H36" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="K36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="3" t="n">
-        <v>45021.8342476852</v>
+        <v>45021</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>1</v>
@@ -1847,14 +1887,15 @@
       <c r="H37" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="K37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="3" t="n">
-        <v>45033.285625</v>
+        <v>45033</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>1</v>
@@ -1874,14 +1915,15 @@
       <c r="H38" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="K38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B39" s="3" t="n">
-        <v>45095.1629513889</v>
+        <v>45095</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>0</v>
@@ -1901,14 +1943,15 @@
       <c r="H39" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="K39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="3" t="n">
-        <v>45112.6531018519</v>
+        <v>45112</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>0</v>
@@ -1928,14 +1971,15 @@
       <c r="H40" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="K40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B41" s="3" t="n">
-        <v>45124.1045023148</v>
+        <v>45124</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>0</v>
@@ -1955,14 +1999,15 @@
       <c r="H41" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="K41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="3" t="n">
-        <v>45174.530462963</v>
+        <v>45174</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>0</v>
@@ -1982,14 +2027,15 @@
       <c r="H42" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="K42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B43" s="3" t="n">
-        <v>45203.4721759259</v>
+        <v>45203</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>0</v>
@@ -2009,14 +2055,15 @@
       <c r="H43" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="K43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="3" t="n">
-        <v>45294.291412037</v>
+        <v>45294</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>1</v>
@@ -2036,14 +2083,15 @@
       <c r="H44" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="K44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B45" s="3" t="n">
-        <v>45305.7427777778</v>
+        <v>45305</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>1</v>
@@ -2063,14 +2111,15 @@
       <c r="H45" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="K45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B46" s="3" t="n">
-        <v>45367.6201388889</v>
+        <v>45367</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>1</v>
@@ -2090,14 +2139,15 @@
       <c r="H46" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="K46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="3" t="n">
-        <v>45385.1103935185</v>
+        <v>45385</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>1</v>
@@ -2117,14 +2167,15 @@
       <c r="H47" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="K47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B48" s="3" t="n">
-        <v>45389.1046180556</v>
+        <v>45389</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>1</v>
@@ -2144,14 +2195,15 @@
       <c r="H48" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="K48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B49" s="3" t="n">
-        <v>45396.5618171296</v>
+        <v>45396</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>1</v>
@@ -2171,14 +2223,15 @@
       <c r="H49" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="K49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B50" s="3" t="n">
-        <v>45487.3810069444</v>
+        <v>45487</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>0</v>
@@ -2198,7 +2251,8 @@
       <c r="H50" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="K50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="K50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
@@ -2225,14 +2279,15 @@
       <c r="H51" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="K51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B52" s="3" t="n">
-        <v>43419.4984722222</v>
+        <v>43419</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>1</v>
@@ -2252,14 +2307,15 @@
       <c r="H52" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="K52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="3" t="n">
-        <v>43591.6351851852</v>
+        <v>43591</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>0</v>
@@ -2279,14 +2335,15 @@
       <c r="H53" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="K53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B54" s="3" t="n">
-        <v>43601.1369560185</v>
+        <v>43601</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>0</v>
@@ -2306,14 +2363,15 @@
       <c r="H54" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="K54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B55" s="3" t="n">
-        <v>43720.8979398148</v>
+        <v>43720</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>0</v>
@@ -2333,14 +2391,15 @@
       <c r="H55" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="K55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B56" s="3" t="n">
-        <v>43835.1513657407</v>
+        <v>43835</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>1</v>
@@ -2360,14 +2419,15 @@
       <c r="H56" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="K56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B57" s="3" t="n">
-        <v>43902.5365625</v>
+        <v>43902</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>1</v>
@@ -2387,14 +2447,15 @@
       <c r="H57" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="K57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B58" s="3" t="n">
-        <v>43954.9123611111</v>
+        <v>43954</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>0.3</v>
@@ -2414,14 +2475,15 @@
       <c r="H58" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="K58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B59" s="3" t="n">
-        <v>43964.4141666667</v>
+        <v>43964</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>0</v>
@@ -2441,14 +2503,15 @@
       <c r="H59" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="K59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B60" s="3" t="n">
-        <v>44016.7899421296</v>
+        <v>44016</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>0</v>
@@ -2468,14 +2531,15 @@
       <c r="H60" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="K60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B61" s="3" t="n">
-        <v>44055.2334375</v>
+        <v>44055</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>0</v>
@@ -2495,14 +2559,15 @@
       <c r="H61" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="K61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B62" s="3" t="n">
-        <v>44136.5509722222</v>
+        <v>44136</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>1</v>
@@ -2522,14 +2587,15 @@
       <c r="H62" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="K62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B63" s="3" t="n">
-        <v>44146.0527546296</v>
+        <v>44146</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>1</v>
@@ -2549,14 +2615,15 @@
       <c r="H63" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="K63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B64" s="3" t="n">
-        <v>44198.4286226852</v>
+        <v>44198</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>1</v>
@@ -2576,14 +2643,15 @@
       <c r="H64" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="K64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B65" s="3" t="n">
-        <v>44236.8721412037</v>
+        <v>44236</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>1</v>
@@ -2603,14 +2671,15 @@
       <c r="H65" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="K65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B66" s="3" t="n">
-        <v>44318.1896759259</v>
+        <v>44318</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>0.3</v>
@@ -2630,14 +2699,15 @@
       <c r="H66" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="K66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B67" s="3" t="n">
-        <v>44327.6914814815</v>
+        <v>44327</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>0</v>
@@ -2657,14 +2727,15 @@
       <c r="H67" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="K67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B68" s="3" t="n">
-        <v>44409.0090277778</v>
+        <v>44409</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>0</v>
@@ -2684,14 +2755,15 @@
       <c r="H68" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="K68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B69" s="3" t="n">
-        <v>44681.4671180556</v>
+        <v>44681</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>0.9</v>
@@ -2711,14 +2783,15 @@
       <c r="H69" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="K69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B70" s="3" t="n">
-        <v>44690.9688773148</v>
+        <v>44690</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>0.7</v>
@@ -2738,14 +2811,15 @@
       <c r="H70" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="K70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B71" s="3" t="n">
-        <v>44772.2865972222</v>
+        <v>44772</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>0</v>
@@ -2765,14 +2839,15 @@
       <c r="H71" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="K71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B72" s="3" t="n">
-        <v>44863.1058449074</v>
+        <v>44863</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>1</v>
@@ -2792,14 +2867,15 @@
       <c r="H72" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="K72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B73" s="3" t="n">
-        <v>44953.9251736111</v>
+        <v>44953</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>1</v>
@@ -2819,14 +2895,15 @@
       <c r="H73" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="K73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B74" s="3" t="n">
-        <v>44963.4269444444</v>
+        <v>44963</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>1</v>
@@ -2846,14 +2923,15 @@
       <c r="H74" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="K74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="K74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B75" s="3" t="n">
-        <v>45044.744375</v>
+        <v>45044</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>1</v>
@@ -2873,13 +2951,14 @@
       <c r="H75" s="0" t="n">
         <v>504</v>
       </c>
+      <c r="I75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B76" s="3" t="n">
-        <v>45054.2461805556</v>
+        <v>45054</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>0.8</v>
@@ -2899,13 +2978,14 @@
       <c r="H76" s="0" t="n">
         <v>504</v>
       </c>
+      <c r="I76" s="5"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B77" s="3" t="n">
-        <v>45135.563275463</v>
+        <v>45135</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>0</v>
@@ -2925,13 +3005,14 @@
       <c r="H77" s="0" t="n">
         <v>504</v>
       </c>
+      <c r="I77" s="5"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B78" s="3" t="n">
-        <v>45145.0650462963</v>
+        <v>45145</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>0</v>
@@ -2951,13 +3032,14 @@
       <c r="H78" s="0" t="n">
         <v>504</v>
       </c>
+      <c r="I78" s="5"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B79" s="3" t="n">
-        <v>45197.4407060185</v>
+        <v>45197</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>0.5</v>
@@ -2977,13 +3059,14 @@
       <c r="H79" s="0" t="n">
         <v>504</v>
       </c>
+      <c r="I79" s="5"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B80" s="3" t="n">
-        <v>45226.3825810185</v>
+        <v>45226</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>1</v>
@@ -3003,13 +3086,14 @@
       <c r="H80" s="0" t="n">
         <v>504</v>
       </c>
+      <c r="I80" s="5"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B81" s="3" t="n">
-        <v>45317.2014930556</v>
+        <v>45317</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>1</v>
@@ -3027,13 +3111,14 @@
       <c r="H81" s="0" t="n">
         <v>504</v>
       </c>
+      <c r="I81" s="5"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B82" s="3" t="n">
-        <v>45408.0205439815</v>
+        <v>45408</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>0.3</v>
@@ -3053,13 +3138,14 @@
       <c r="H82" s="0" t="n">
         <v>504</v>
       </c>
+      <c r="I82" s="5"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B83" s="3" t="n">
-        <v>45498.8398032407</v>
+        <v>45498</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>0</v>
@@ -3079,13 +3165,14 @@
       <c r="H83" s="0" t="n">
         <v>504</v>
       </c>
+      <c r="I83" s="5"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B84" s="3" t="n">
-        <v>43408.370775463</v>
+        <v>43408</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>0</v>
@@ -3105,13 +3192,14 @@
       <c r="H84" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I84" s="5"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B85" s="3" t="n">
-        <v>43550.5740277778</v>
+        <v>43550</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>1</v>
@@ -3131,13 +3219,14 @@
       <c r="H85" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I85" s="5"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B86" s="3" t="n">
-        <v>43732.2125810185</v>
+        <v>43732</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>0</v>
@@ -3157,13 +3246,14 @@
       <c r="H86" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I86" s="5"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B87" s="3" t="n">
-        <v>43823.031875</v>
+        <v>43823</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>1</v>
@@ -3183,13 +3273,14 @@
       <c r="H87" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I87" s="5"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B88" s="3" t="n">
-        <v>43862.4671990741</v>
+        <v>43862</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>1</v>
@@ -3209,13 +3300,14 @@
       <c r="H88" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I88" s="5"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B89" s="3" t="n">
-        <v>43953.2864814815</v>
+        <v>43953</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>0</v>
@@ -3235,13 +3327,14 @@
       <c r="H89" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I89" s="5"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B90" s="3" t="n">
-        <v>44004.6704398148</v>
+        <v>44004</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>0</v>
@@ -3261,13 +3354,14 @@
       <c r="H90" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I90" s="5"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B91" s="3" t="n">
-        <v>44044.105787037</v>
+        <v>44044</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>0</v>
@@ -3287,13 +3381,14 @@
       <c r="H91" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I91" s="5"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B92" s="3" t="n">
-        <v>44095.4897569444</v>
+        <v>44095</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>0</v>
@@ -3313,13 +3408,14 @@
       <c r="H92" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I92" s="5"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B93" s="3" t="n">
-        <v>44134.9251041667</v>
+        <v>44134</v>
       </c>
       <c r="C93" s="1" t="n">
         <v>0.8</v>
@@ -3339,13 +3435,14 @@
       <c r="H93" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I93" s="5"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B94" s="3" t="n">
-        <v>44225.7444791667</v>
+        <v>44225</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>1</v>
@@ -3365,13 +3462,14 @@
       <c r="H94" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I94" s="5"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B95" s="3" t="n">
-        <v>44248.1867592593</v>
+        <v>44248</v>
       </c>
       <c r="C95" s="1" t="n">
         <v>1</v>
@@ -3391,13 +3489,14 @@
       <c r="H95" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I95" s="5"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B96" s="3" t="n">
-        <v>44316.5637962963</v>
+        <v>44316</v>
       </c>
       <c r="C96" s="1" t="n">
         <v>0</v>
@@ -3417,13 +3516,14 @@
       <c r="H96" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I96" s="5"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B97" s="3" t="n">
-        <v>44407.3831712963</v>
+        <v>44407</v>
       </c>
       <c r="C97" s="1" t="n">
         <v>0</v>
@@ -3443,13 +3543,14 @@
       <c r="H97" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I97" s="5"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B98" s="3" t="n">
-        <v>44458.7671875</v>
+        <v>44458</v>
       </c>
       <c r="C98" s="1" t="n">
         <v>0</v>
@@ -3469,13 +3570,14 @@
       <c r="H98" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I98" s="5"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B99" s="3" t="n">
-        <v>44520.6449074074</v>
+        <v>44520</v>
       </c>
       <c r="C99" s="1" t="n">
         <v>0.9</v>
@@ -3495,13 +3597,14 @@
       <c r="H99" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I99" s="5"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B100" s="3" t="n">
-        <v>44640.4059375</v>
+        <v>44640</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>1</v>
@@ -3521,13 +3624,14 @@
       <c r="H100" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I100" s="5"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B101" s="3" t="n">
-        <v>44731.2253009259</v>
+        <v>44731</v>
       </c>
       <c r="C101" s="1" t="n">
         <v>0</v>
@@ -3547,13 +3651,14 @@
       <c r="H101" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I101" s="5"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B102" s="3" t="n">
-        <v>44770.6606944444</v>
+        <v>44770</v>
       </c>
       <c r="C102" s="1" t="n">
         <v>0</v>
@@ -3573,13 +3678,14 @@
       <c r="H102" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I102" s="5"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B103" s="3" t="n">
-        <v>44822.0446875</v>
+        <v>44822</v>
       </c>
       <c r="C103" s="1" t="n">
         <v>0</v>
@@ -3599,13 +3705,14 @@
       <c r="H103" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I103" s="5"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B104" s="3" t="n">
-        <v>44861.4799768519</v>
+        <v>44861</v>
       </c>
       <c r="C104" s="1" t="n">
         <v>0</v>
@@ -3625,13 +3732,14 @@
       <c r="H104" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I104" s="5"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B105" s="3" t="n">
-        <v>44952.2993865741</v>
+        <v>44952</v>
       </c>
       <c r="C105" s="1" t="n">
         <v>1</v>
@@ -3651,13 +3759,14 @@
       <c r="H105" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I105" s="5"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B106" s="3" t="n">
-        <v>45003.6833217593</v>
+        <v>45003</v>
       </c>
       <c r="C106" s="1" t="n">
         <v>1</v>
@@ -3677,13 +3786,14 @@
       <c r="H106" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I106" s="5"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B107" s="3" t="n">
-        <v>45094.5022569444</v>
+        <v>45094</v>
       </c>
       <c r="C107" s="1" t="n">
         <v>0</v>
@@ -3703,13 +3813,14 @@
       <c r="H107" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I107" s="5"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B108" s="3" t="n">
-        <v>45133.9374074074</v>
+        <v>45133</v>
       </c>
       <c r="C108" s="1" t="n">
         <v>0</v>
@@ -3729,13 +3840,14 @@
       <c r="H108" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I108" s="5"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B109" s="3" t="n">
-        <v>45406.3947453704</v>
+        <v>45406</v>
       </c>
       <c r="C109" s="1" t="n">
         <v>0</v>
@@ -3755,13 +3867,14 @@
       <c r="H109" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I109" s="5"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B110" s="3" t="n">
-        <v>45497.2139699074</v>
+        <v>45497</v>
       </c>
       <c r="C110" s="1" t="n">
         <v>0</v>
@@ -3781,13 +3894,14 @@
       <c r="H110" s="0" t="n">
         <v>413</v>
       </c>
+      <c r="I110" s="5"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B111" s="3" t="n">
-        <v>43591.4328472222</v>
+        <v>43591</v>
       </c>
       <c r="C111" s="1" t="n">
         <v>0.2</v>
@@ -3807,13 +3921,14 @@
       <c r="H111" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I111" s="5"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B112" s="3" t="n">
-        <v>43659.8096875</v>
+        <v>43659</v>
       </c>
       <c r="C112" s="1" t="n">
         <v>0</v>
@@ -3833,13 +3948,14 @@
       <c r="H112" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I112" s="5"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B113" s="3" t="n">
-        <v>43688.7514930556</v>
+        <v>43688</v>
       </c>
       <c r="C113" s="1" t="n">
         <v>0</v>
@@ -3859,13 +3975,14 @@
       <c r="H113" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I113" s="5"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B114" s="3" t="n">
-        <v>43711.1937962963</v>
+        <v>43711</v>
       </c>
       <c r="C114" s="1" t="n">
         <v>0</v>
@@ -3885,13 +4002,14 @@
       <c r="H114" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I114" s="5"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B115" s="3" t="n">
-        <v>43802.013125</v>
+        <v>43802</v>
       </c>
       <c r="C115" s="1" t="n">
         <v>2</v>
@@ -3911,13 +4029,14 @@
       <c r="H115" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I115" s="5"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B116" s="3" t="n">
-        <v>43863.8907175926</v>
+        <v>43863</v>
       </c>
       <c r="C116" s="1" t="n">
         <v>1</v>
@@ -3937,13 +4056,14 @@
       <c r="H116" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I116" s="5"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B117" s="3" t="n">
-        <v>43932.2677430556</v>
+        <v>43932</v>
       </c>
       <c r="C117" s="1" t="n">
         <v>1</v>
@@ -3963,13 +4083,14 @@
       <c r="H117" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I117" s="5"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B118" s="3" t="n">
-        <v>43983.651724537</v>
+        <v>43983</v>
       </c>
       <c r="C118" s="1" t="n">
         <v>0</v>
@@ -3989,13 +4110,14 @@
       <c r="H118" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I118" s="5"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B119" s="3" t="n">
-        <v>44023.087025463</v>
+        <v>44023</v>
       </c>
       <c r="C119" s="1" t="n">
         <v>0</v>
@@ -4015,13 +4137,14 @@
       <c r="H119" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I119" s="5"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B120" s="3" t="n">
-        <v>44045.5293171296</v>
+        <v>44045</v>
       </c>
       <c r="C120" s="1" t="n">
         <v>0</v>
@@ -4041,13 +4164,14 @@
       <c r="H120" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I120" s="5"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B121" s="3" t="n">
-        <v>44227.1680092593</v>
+        <v>44227</v>
       </c>
       <c r="C121" s="1" t="n">
         <v>1</v>
@@ -4067,13 +4191,14 @@
       <c r="H121" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I121" s="5"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B122" s="3" t="n">
-        <v>44233.6674421296</v>
+        <v>44233</v>
       </c>
       <c r="C122" s="1" t="n">
         <v>1</v>
@@ -4093,13 +4218,14 @@
       <c r="H122" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I122" s="5"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B123" s="3" t="n">
-        <v>44295.5450578704</v>
+        <v>44295</v>
       </c>
       <c r="C123" s="1" t="n">
         <v>0.3</v>
@@ -4119,13 +4245,14 @@
       <c r="H123" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I123" s="5"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B124" s="3" t="n">
-        <v>44408.8066898148</v>
+        <v>44408</v>
       </c>
       <c r="C124" s="1" t="n">
         <v>0</v>
@@ -4145,13 +4272,14 @@
       <c r="H124" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I124" s="5"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B125" s="3" t="n">
-        <v>44710.2065509259</v>
+        <v>44710</v>
       </c>
       <c r="C125" s="1" t="n">
         <v>0</v>
@@ -4171,13 +4299,14 @@
       <c r="H125" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I125" s="5"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B126" s="3" t="n">
-        <v>44749.6419560185</v>
+        <v>44749</v>
       </c>
       <c r="C126" s="1" t="n">
         <v>0</v>
@@ -4197,13 +4326,14 @@
       <c r="H126" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I126" s="5"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B127" s="3" t="n">
-        <v>44801.0259953704</v>
+        <v>44801</v>
       </c>
       <c r="C127" s="1" t="n">
         <v>0</v>
@@ -4223,13 +4353,14 @@
       <c r="H127" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I127" s="5"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B128" s="3" t="n">
-        <v>44840.4611921296</v>
+        <v>44840</v>
       </c>
       <c r="C128" s="1" t="n">
         <v>0</v>
@@ -4249,13 +4380,14 @@
       <c r="H128" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I128" s="5"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B129" s="3" t="n">
-        <v>44862.9034837963</v>
+        <v>44862</v>
       </c>
       <c r="C129" s="1" t="n">
         <v>0</v>
@@ -4275,13 +4407,14 @@
       <c r="H129" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I129" s="5"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B130" s="3" t="n">
-        <v>44953.7228125</v>
+        <v>44953</v>
       </c>
       <c r="E130" s="4"/>
       <c r="F130" s="0" t="n">
@@ -4293,13 +4426,14 @@
       <c r="H130" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I130" s="5"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B131" s="3" t="n">
-        <v>45112.9187731482</v>
+        <v>45112</v>
       </c>
       <c r="C131" s="1" t="n">
         <v>0</v>
@@ -4319,13 +4453,14 @@
       <c r="H131" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I131" s="5"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B132" s="3" t="n">
-        <v>45203.7378703704</v>
+        <v>45203</v>
       </c>
       <c r="C132" s="1" t="n">
         <v>0</v>
@@ -4345,13 +4480,14 @@
       <c r="H132" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I132" s="5"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B133" s="3" t="n">
-        <v>45385.3760648148</v>
+        <v>45385</v>
       </c>
       <c r="C133" s="1" t="n">
         <v>1</v>
@@ -4371,13 +4507,14 @@
       <c r="H133" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I133" s="5"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>119</v>
       </c>
       <c r="B134" s="3" t="n">
-        <v>45476.1953587963</v>
+        <v>45476</v>
       </c>
       <c r="C134" s="1" t="n">
         <v>0</v>
@@ -4397,13 +4534,14 @@
       <c r="H134" s="0" t="n">
         <v>313</v>
       </c>
+      <c r="I134" s="5"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B135" s="3" t="n">
-        <v>43434.0383796296</v>
+        <v>43434</v>
       </c>
       <c r="C135" s="1" t="n">
         <v>1</v>
@@ -4423,14 +4561,15 @@
       <c r="H135" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K135" s="5"/>
+      <c r="I135" s="5"/>
+      <c r="K135" s="6"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B136" s="3" t="n">
-        <v>43518.3584143519</v>
+        <v>43518</v>
       </c>
       <c r="C136" s="1" t="n">
         <v>1</v>
@@ -4450,14 +4589,15 @@
       <c r="H136" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K136" s="5"/>
+      <c r="I136" s="5"/>
+      <c r="K136" s="6"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B137" s="3" t="n">
-        <v>43524.8578472222</v>
+        <v>43524</v>
       </c>
       <c r="C137" s="1" t="n">
         <v>0.8</v>
@@ -4477,14 +4617,15 @@
       <c r="H137" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K137" s="5"/>
+      <c r="I137" s="5"/>
+      <c r="K137" s="6"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B138" s="3" t="n">
-        <v>43609.1775925926</v>
+        <v>43609</v>
       </c>
       <c r="C138" s="1" t="n">
         <v>0.1</v>
@@ -4504,14 +4645,15 @@
       <c r="H138" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K138" s="5"/>
+      <c r="I138" s="5"/>
+      <c r="K138" s="6"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B139" s="3" t="n">
-        <v>43615.6770023148</v>
+        <v>43615</v>
       </c>
       <c r="C139" s="1" t="n">
         <v>0</v>
@@ -4531,14 +4673,15 @@
       <c r="H139" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K139" s="5"/>
+      <c r="I139" s="5"/>
+      <c r="K139" s="6"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B140" s="3" t="n">
-        <v>43735.4380671296</v>
+        <v>43735</v>
       </c>
       <c r="C140" s="1" t="n">
         <v>0</v>
@@ -4558,14 +4701,15 @@
       <c r="H140" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K140" s="5"/>
+      <c r="I140" s="5"/>
+      <c r="K140" s="6"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B141" s="3" t="n">
-        <v>43881.6355092593</v>
+        <v>43881</v>
       </c>
       <c r="C141" s="1" t="n">
         <v>1</v>
@@ -4585,14 +4729,15 @@
       <c r="H141" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K141" s="5"/>
+      <c r="I141" s="5"/>
+      <c r="K141" s="6"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B142" s="3" t="n">
-        <v>43888.1349189815</v>
+        <v>43888</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>1</v>
@@ -4612,14 +4757,15 @@
       <c r="H142" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K142" s="5"/>
+      <c r="I142" s="5"/>
+      <c r="K142" s="6"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B143" s="3" t="n">
-        <v>43972.454837963</v>
+        <v>43972</v>
       </c>
       <c r="C143" s="1" t="n">
         <v>0</v>
@@ -4639,14 +4785,15 @@
       <c r="H143" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K143" s="5"/>
+      <c r="I143" s="5"/>
+      <c r="K143" s="6"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B144" s="3" t="n">
-        <v>44063.2741087963</v>
+        <v>44063</v>
       </c>
       <c r="C144" s="1" t="n">
         <v>0</v>
@@ -4666,14 +4813,15 @@
       <c r="H144" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K144" s="5"/>
+      <c r="I144" s="5"/>
+      <c r="K144" s="6"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B145" s="3" t="n">
-        <v>44069.7735300926</v>
+        <v>44069</v>
       </c>
       <c r="C145" s="1" t="n">
         <v>0</v>
@@ -4693,14 +4841,15 @@
       <c r="H145" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K145" s="5"/>
+      <c r="I145" s="5"/>
+      <c r="K145" s="6"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B146" s="3" t="n">
-        <v>44154.0934259259</v>
+        <v>44154</v>
       </c>
       <c r="C146" s="1" t="n">
         <v>0</v>
@@ -4720,14 +4869,15 @@
       <c r="H146" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K146" s="5"/>
+      <c r="I146" s="5"/>
+      <c r="K146" s="6"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B147" s="3" t="n">
-        <v>44160.5928703704</v>
+        <v>44160</v>
       </c>
       <c r="C147" s="1" t="n">
         <v>0</v>
@@ -4747,14 +4897,15 @@
       <c r="H147" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K147" s="5"/>
+      <c r="I147" s="5"/>
+      <c r="K147" s="6"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B148" s="3" t="n">
-        <v>44244.9128009259</v>
+        <v>44244</v>
       </c>
       <c r="C148" s="1" t="n">
         <v>1</v>
@@ -4774,14 +4925,15 @@
       <c r="H148" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K148" s="5"/>
+      <c r="I148" s="5"/>
+      <c r="K148" s="6"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B149" s="3" t="n">
-        <v>44342.2315625</v>
+        <v>44342</v>
       </c>
       <c r="C149" s="1" t="n">
         <v>0</v>
@@ -4801,14 +4953,15 @@
       <c r="H149" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K149" s="5"/>
+      <c r="I149" s="5"/>
+      <c r="K149" s="6"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B150" s="3" t="n">
-        <v>44426.5515162037</v>
+        <v>44426</v>
       </c>
       <c r="C150" s="1" t="n">
         <v>0</v>
@@ -4828,14 +4981,15 @@
       <c r="H150" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K150" s="5"/>
+      <c r="I150" s="5"/>
+      <c r="K150" s="6"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B151" s="3" t="n">
-        <v>44433.0509490741</v>
+        <v>44433</v>
       </c>
       <c r="C151" s="1" t="n">
         <v>0</v>
@@ -4855,14 +5009,15 @@
       <c r="H151" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K151" s="5"/>
+      <c r="I151" s="5"/>
+      <c r="K151" s="6"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B152" s="3" t="n">
-        <v>44608.1902430556</v>
+        <v>44608</v>
       </c>
       <c r="C152" s="1" t="n">
         <v>0.7</v>
@@ -4882,14 +5037,15 @@
       <c r="H152" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K152" s="5"/>
+      <c r="I152" s="5"/>
+      <c r="K152" s="6"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B153" s="3" t="n">
-        <v>44614.6896990741</v>
+        <v>44614</v>
       </c>
       <c r="C153" s="1" t="n">
         <v>1</v>
@@ -4909,14 +5065,15 @@
       <c r="H153" s="0" t="n">
         <v>2091</v>
       </c>
-      <c r="K153" s="5"/>
+      <c r="I153" s="5"/>
+      <c r="K153" s="6"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B154" s="3" t="n">
-        <v>44705.5090046296</v>
+        <v>44705</v>
       </c>
       <c r="C154" s="1" t="n">
         <v>0</v>
@@ -4936,13 +5093,14 @@
       <c r="H154" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I154" s="5"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B155" s="3" t="n">
-        <v>44789.8290393519</v>
+        <v>44789</v>
       </c>
       <c r="C155" s="1" t="n">
         <v>0</v>
@@ -4962,13 +5120,14 @@
       <c r="H155" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I155" s="5"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B156" s="3" t="n">
-        <v>44796.3284953704</v>
+        <v>44796</v>
       </c>
       <c r="C156" s="1" t="n">
         <v>0</v>
@@ -4988,13 +5147,14 @@
       <c r="H156" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I156" s="5"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B157" s="3" t="n">
-        <v>44971.4676041667</v>
+        <v>44971</v>
       </c>
       <c r="C157" s="1" t="n">
         <v>1</v>
@@ -5012,13 +5172,14 @@
       <c r="H157" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I157" s="5"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B158" s="3" t="n">
-        <v>44977.9670023148</v>
+        <v>44977</v>
       </c>
       <c r="C158" s="1" t="n">
         <v>1</v>
@@ -5036,13 +5197,14 @@
       <c r="H158" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I158" s="5"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B159" s="3" t="n">
-        <v>45062.2867824074</v>
+        <v>45062</v>
       </c>
       <c r="C159" s="1" t="n">
         <v>0</v>
@@ -5060,13 +5222,14 @@
       <c r="H159" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I159" s="5"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B160" s="3" t="n">
-        <v>45068.7862152778</v>
+        <v>45068</v>
       </c>
       <c r="C160" s="1" t="n">
         <v>0</v>
@@ -5084,13 +5247,14 @@
       <c r="H160" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I160" s="5"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B161" s="3" t="n">
-        <v>45153.1056944444</v>
+        <v>45153</v>
       </c>
       <c r="C161" s="1" t="n">
         <v>0</v>
@@ -5108,13 +5272,14 @@
       <c r="H161" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I161" s="5"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B162" s="3" t="n">
-        <v>45159.6050462963</v>
+        <v>45159</v>
       </c>
       <c r="C162" s="1" t="n">
         <v>0</v>
@@ -5132,13 +5297,14 @@
       <c r="H162" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I162" s="5"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B163" s="3" t="n">
-        <v>45243.9248958333</v>
+        <v>45243</v>
       </c>
       <c r="C163" s="1" t="n">
         <v>0</v>
@@ -5156,13 +5322,14 @@
       <c r="H163" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I163" s="5"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B164" s="3" t="n">
-        <v>45250.4243865741</v>
+        <v>45250</v>
       </c>
       <c r="E164" s="4"/>
       <c r="F164" s="0" t="n">
@@ -5174,13 +5341,14 @@
       <c r="H164" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I164" s="5"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B165" s="3" t="n">
-        <v>45334.7439351852</v>
+        <v>45334</v>
       </c>
       <c r="E165" s="4"/>
       <c r="F165" s="0" t="n">
@@ -5192,13 +5360,14 @@
       <c r="H165" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I165" s="5"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B166" s="3" t="n">
-        <v>45341.2433564815</v>
+        <v>45341</v>
       </c>
       <c r="E166" s="4"/>
       <c r="F166" s="0" t="n">
@@ -5210,13 +5379,14 @@
       <c r="H166" s="0" t="n">
         <v>2091</v>
       </c>
+      <c r="I166" s="5"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B167" s="3" t="n">
-        <v>43490.2849305556</v>
+        <v>43490</v>
       </c>
       <c r="C167" s="1" t="n">
         <v>0.1</v>
@@ -5236,14 +5406,15 @@
       <c r="H167" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K167" s="5"/>
+      <c r="I167" s="5"/>
+      <c r="K167" s="6"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B168" s="3" t="n">
-        <v>43636.4822916667</v>
+        <v>43636</v>
       </c>
       <c r="C168" s="1" t="n">
         <v>0</v>
@@ -5263,14 +5434,15 @@
       <c r="H168" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K168" s="5"/>
+      <c r="I168" s="5"/>
+      <c r="K168" s="6"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B169" s="3" t="n">
-        <v>43671.9233680556</v>
+        <v>43671</v>
       </c>
       <c r="C169" s="1" t="n">
         <v>0</v>
@@ -5290,14 +5462,15 @@
       <c r="H169" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K169" s="5"/>
+      <c r="I169" s="5"/>
+      <c r="K169" s="6"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B170" s="3" t="n">
-        <v>43700.8651388889</v>
+        <v>43700</v>
       </c>
       <c r="C170" s="1" t="n">
         <v>0</v>
@@ -5317,14 +5490,15 @@
       <c r="H170" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K170" s="5"/>
+      <c r="I170" s="5"/>
+      <c r="K170" s="6"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B171" s="3" t="n">
-        <v>43727.3016319444</v>
+        <v>43727</v>
       </c>
       <c r="C171" s="1" t="n">
         <v>0</v>
@@ -5344,14 +5518,15 @@
       <c r="H171" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K171" s="5"/>
+      <c r="I171" s="5"/>
+      <c r="K171" s="6"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B172" s="3" t="n">
-        <v>43762.7428009259</v>
+        <v>43762</v>
       </c>
       <c r="C172" s="1" t="n">
         <v>0</v>
@@ -5368,14 +5543,15 @@
       <c r="H172" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K172" s="5"/>
+      <c r="I172" s="5"/>
+      <c r="K172" s="6"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B173" s="3" t="n">
-        <v>43853.5620601852</v>
+        <v>43853</v>
       </c>
       <c r="C173" s="1" t="n">
         <v>0.8</v>
@@ -5395,14 +5571,15 @@
       <c r="H173" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K173" s="5"/>
+      <c r="I173" s="5"/>
+      <c r="K173" s="6"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B174" s="3" t="n">
-        <v>43879.9985300926</v>
+        <v>43879</v>
       </c>
       <c r="C174" s="1" t="n">
         <v>0</v>
@@ -5422,14 +5599,15 @@
       <c r="H174" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K174" s="5"/>
+      <c r="I174" s="5"/>
+      <c r="K174" s="6"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B175" s="3" t="n">
-        <v>43944.3813888889</v>
+        <v>43944</v>
       </c>
       <c r="C175" s="1" t="n">
         <v>0</v>
@@ -5449,14 +5627,15 @@
       <c r="H175" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K175" s="5"/>
+      <c r="I175" s="5"/>
+      <c r="K175" s="6"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B176" s="3" t="n">
-        <v>43999.759525463</v>
+        <v>43999</v>
       </c>
       <c r="C176" s="1" t="n">
         <v>0</v>
@@ -5476,14 +5655,15 @@
       <c r="H176" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K176" s="5"/>
+      <c r="I176" s="5"/>
+      <c r="K176" s="6"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B177" s="3" t="n">
-        <v>44035.2006597222</v>
+        <v>44035</v>
       </c>
       <c r="C177" s="1" t="n">
         <v>0</v>
@@ -5503,14 +5683,15 @@
       <c r="H177" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K177" s="5"/>
+      <c r="I177" s="5"/>
+      <c r="K177" s="6"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B178" s="3" t="n">
-        <v>44126.0199421296</v>
+        <v>44126</v>
       </c>
       <c r="C178" s="1" t="n">
         <v>0</v>
@@ -5530,14 +5711,15 @@
       <c r="H178" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K178" s="5"/>
+      <c r="I178" s="5"/>
+      <c r="K178" s="6"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B179" s="3" t="n">
-        <v>44243.2758217593</v>
+        <v>44243</v>
       </c>
       <c r="C179" s="1" t="n">
         <v>1</v>
@@ -5557,14 +5739,15 @@
       <c r="H179" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K179" s="5"/>
+      <c r="I179" s="5"/>
+      <c r="K179" s="6"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B180" s="3" t="n">
-        <v>44307.6586689815</v>
+        <v>44307</v>
       </c>
       <c r="C180" s="1" t="n">
         <v>0</v>
@@ -5584,14 +5767,15 @@
       <c r="H180" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K180" s="5"/>
+      <c r="I180" s="5"/>
+      <c r="K180" s="6"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B181" s="3" t="n">
-        <v>44363.0368634259</v>
+        <v>44363</v>
       </c>
       <c r="C181" s="1" t="n">
         <v>0</v>
@@ -5611,14 +5795,15 @@
       <c r="H181" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K181" s="5"/>
+      <c r="I181" s="5"/>
+      <c r="K181" s="6"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B182" s="3" t="n">
-        <v>44398.4780092593</v>
+        <v>44398</v>
       </c>
       <c r="C182" s="1" t="n">
         <v>0</v>
@@ -5638,14 +5823,15 @@
       <c r="H182" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K182" s="5"/>
+      <c r="I182" s="5"/>
+      <c r="K182" s="6"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B183" s="3" t="n">
-        <v>44453.8562615741</v>
+        <v>44453</v>
       </c>
       <c r="C183" s="1" t="n">
         <v>0</v>
@@ -5665,14 +5851,15 @@
       <c r="H183" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K183" s="5"/>
+      <c r="I183" s="5"/>
+      <c r="K183" s="6"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B184" s="3" t="n">
-        <v>44515.7339699074</v>
+        <v>44515</v>
       </c>
       <c r="C184" s="1" t="n">
         <v>0</v>
@@ -5689,14 +5876,15 @@
       <c r="H184" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K184" s="5"/>
+      <c r="I184" s="5"/>
+      <c r="K184" s="6"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B185" s="3" t="n">
-        <v>44580.1168055556</v>
+        <v>44580</v>
       </c>
       <c r="C185" s="1" t="n">
         <v>0.7</v>
@@ -5716,14 +5904,15 @@
       <c r="H185" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K185" s="5"/>
+      <c r="I185" s="5"/>
+      <c r="K185" s="6"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B186" s="3" t="n">
-        <v>44670.936099537</v>
+        <v>44670</v>
       </c>
       <c r="C186" s="1" t="n">
         <v>0</v>
@@ -5743,14 +5932,15 @@
       <c r="H186" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K186" s="5"/>
+      <c r="I186" s="5"/>
+      <c r="K186" s="6"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B187" s="3" t="n">
-        <v>44726.3143518519</v>
+        <v>44726</v>
       </c>
       <c r="C187" s="1" t="n">
         <v>0</v>
@@ -5770,14 +5960,15 @@
       <c r="H187" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K187" s="5"/>
+      <c r="I187" s="5"/>
+      <c r="K187" s="6"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B188" s="3" t="n">
-        <v>44761.7555555556</v>
+        <v>44761</v>
       </c>
       <c r="C188" s="1" t="n">
         <v>0</v>
@@ -5797,14 +5988,15 @@
       <c r="H188" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K188" s="5"/>
+      <c r="I188" s="5"/>
+      <c r="K188" s="6"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B189" s="3" t="n">
-        <v>44817.1337731482</v>
+        <v>44817</v>
       </c>
       <c r="C189" s="1" t="n">
         <v>0</v>
@@ -5824,14 +6016,15 @@
       <c r="H189" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K189" s="5"/>
+      <c r="I189" s="5"/>
+      <c r="K189" s="6"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B190" s="3" t="n">
-        <v>44943.3940625</v>
+        <v>44943</v>
       </c>
       <c r="E190" s="4"/>
       <c r="F190" s="0" t="n">
@@ -5843,14 +6036,15 @@
       <c r="H190" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K190" s="5"/>
+      <c r="I190" s="5"/>
+      <c r="K190" s="6"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B191" s="3" t="n">
-        <v>45034.2133564815</v>
+        <v>45034</v>
       </c>
       <c r="F191" s="0" t="n">
         <v>-121.606</v>
@@ -5861,14 +6055,15 @@
       <c r="H191" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K191" s="5"/>
+      <c r="I191" s="5"/>
+      <c r="K191" s="6"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B192" s="3" t="n">
-        <v>45089.5913310185</v>
+        <v>45089</v>
       </c>
       <c r="C192" s="1" t="n">
         <v>0</v>
@@ -5888,14 +6083,15 @@
       <c r="H192" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K192" s="5"/>
+      <c r="I192" s="5"/>
+      <c r="K192" s="6"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B193" s="3" t="n">
-        <v>45125.0323148148</v>
+        <v>45125</v>
       </c>
       <c r="C193" s="1" t="n">
         <v>0</v>
@@ -5915,14 +6111,15 @@
       <c r="H193" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K193" s="5"/>
+      <c r="I193" s="5"/>
+      <c r="K193" s="6"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B194" s="3" t="n">
-        <v>45362.048587963</v>
+        <v>45362</v>
       </c>
       <c r="C194" s="1" t="n">
         <v>0.7</v>
@@ -5942,14 +6139,15 @@
       <c r="H194" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K194" s="5"/>
+      <c r="I194" s="5"/>
+      <c r="K194" s="6"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B195" s="3" t="n">
-        <v>45397.4896296296</v>
+        <v>45397</v>
       </c>
       <c r="C195" s="1" t="n">
         <v>0</v>
@@ -5969,14 +6167,15 @@
       <c r="H195" s="0" t="n">
         <v>977</v>
       </c>
-      <c r="K195" s="5"/>
+      <c r="I195" s="5"/>
+      <c r="K195" s="6"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
         <v>166</v>
       </c>
       <c r="B196" s="3" t="n">
-        <v>45488.3087847222</v>
+        <v>45488</v>
       </c>
       <c r="C196" s="1" t="n">
         <v>0</v>
@@ -5996,6 +6195,7 @@
       <c r="H196" s="0" t="n">
         <v>977</v>
       </c>
+      <c r="I196" s="5"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="3"/>
@@ -6011,163 +6211,163 @@
       <c r="B200" s="3"/>
     </row>
     <row r="204" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K204" s="5"/>
+      <c r="K204" s="6"/>
     </row>
     <row r="205" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K205" s="5"/>
+      <c r="K205" s="6"/>
     </row>
     <row r="206" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K206" s="5"/>
+      <c r="K206" s="6"/>
     </row>
     <row r="207" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K207" s="5"/>
+      <c r="K207" s="6"/>
     </row>
     <row r="208" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K208" s="5"/>
+      <c r="K208" s="6"/>
     </row>
     <row r="209" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K209" s="5"/>
+      <c r="K209" s="6"/>
     </row>
     <row r="210" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K210" s="5"/>
+      <c r="K210" s="6"/>
     </row>
     <row r="211" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K211" s="5"/>
+      <c r="K211" s="6"/>
     </row>
     <row r="212" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K212" s="5"/>
+      <c r="K212" s="6"/>
     </row>
     <row r="213" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K213" s="5"/>
+      <c r="K213" s="6"/>
     </row>
     <row r="214" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K214" s="5"/>
+      <c r="K214" s="6"/>
     </row>
     <row r="215" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K215" s="5"/>
+      <c r="K215" s="6"/>
     </row>
     <row r="216" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K216" s="5"/>
+      <c r="K216" s="6"/>
     </row>
     <row r="217" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K217" s="5"/>
+      <c r="K217" s="6"/>
     </row>
     <row r="218" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K218" s="5"/>
+      <c r="K218" s="6"/>
     </row>
     <row r="219" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K219" s="5"/>
+      <c r="K219" s="6"/>
     </row>
     <row r="220" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K220" s="5"/>
+      <c r="K220" s="6"/>
     </row>
     <row r="221" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K221" s="5"/>
+      <c r="K221" s="6"/>
     </row>
     <row r="222" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K222" s="5"/>
+      <c r="K222" s="6"/>
     </row>
     <row r="223" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K223" s="5"/>
+      <c r="K223" s="6"/>
     </row>
     <row r="224" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K224" s="5"/>
+      <c r="K224" s="6"/>
     </row>
     <row r="251" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K251" s="5"/>
+      <c r="K251" s="6"/>
     </row>
     <row r="252" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K252" s="5"/>
+      <c r="K252" s="6"/>
     </row>
     <row r="253" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K253" s="5"/>
+      <c r="K253" s="6"/>
     </row>
     <row r="254" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K254" s="5"/>
+      <c r="K254" s="6"/>
     </row>
     <row r="255" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K255" s="5"/>
+      <c r="K255" s="6"/>
     </row>
     <row r="256" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K256" s="5"/>
+      <c r="K256" s="6"/>
     </row>
     <row r="257" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K257" s="5"/>
+      <c r="K257" s="6"/>
     </row>
     <row r="258" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K258" s="5"/>
+      <c r="K258" s="6"/>
     </row>
     <row r="259" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K259" s="5"/>
+      <c r="K259" s="6"/>
     </row>
     <row r="260" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K260" s="5"/>
+      <c r="K260" s="6"/>
     </row>
     <row r="261" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K261" s="5"/>
+      <c r="K261" s="6"/>
     </row>
     <row r="262" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K262" s="5"/>
+      <c r="K262" s="6"/>
     </row>
     <row r="263" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K263" s="5"/>
+      <c r="K263" s="6"/>
     </row>
     <row r="264" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K264" s="5"/>
+      <c r="K264" s="6"/>
     </row>
     <row r="265" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K265" s="5"/>
+      <c r="K265" s="6"/>
     </row>
     <row r="266" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K266" s="5"/>
+      <c r="K266" s="6"/>
     </row>
     <row r="267" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K267" s="5"/>
+      <c r="K267" s="6"/>
     </row>
     <row r="268" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K268" s="5"/>
+      <c r="K268" s="6"/>
     </row>
     <row r="269" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K269" s="5"/>
+      <c r="K269" s="6"/>
     </row>
     <row r="270" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K270" s="5"/>
+      <c r="K270" s="6"/>
     </row>
     <row r="271" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K271" s="5"/>
+      <c r="K271" s="6"/>
     </row>
     <row r="272" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K272" s="5"/>
+      <c r="K272" s="6"/>
     </row>
     <row r="298" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K298" s="5"/>
+      <c r="K298" s="6"/>
     </row>
     <row r="299" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K299" s="5"/>
+      <c r="K299" s="6"/>
     </row>
     <row r="300" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K300" s="5"/>
+      <c r="K300" s="6"/>
     </row>
     <row r="301" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K301" s="5"/>
+      <c r="K301" s="6"/>
     </row>
     <row r="302" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K302" s="5"/>
+      <c r="K302" s="6"/>
     </row>
     <row r="303" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K303" s="5"/>
+      <c r="K303" s="6"/>
     </row>
     <row r="304" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K304" s="5"/>
+      <c r="K304" s="6"/>
     </row>
     <row r="305" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K305" s="5"/>
+      <c r="K305" s="6"/>
     </row>
     <row r="306" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K306" s="5"/>
+      <c r="K306" s="6"/>
     </row>
     <row r="307" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K307" s="5"/>
+      <c r="K307" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
working on accuracy and assessing filtering
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -839,11 +839,11 @@
   </sheetPr>
   <dimension ref="A1:K307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D122" activeCellId="0" sqref="D122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
@@ -4012,10 +4012,10 @@
         <v>43802</v>
       </c>
       <c r="C115" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D115" s="0" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E115" s="4" t="s">
         <v>124</v>
@@ -4177,7 +4177,7 @@
         <v>1</v>
       </c>
       <c r="D121" s="0" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E121" s="4" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
we are in an excellent place with two quality filters, then two sorting filters that are quite logical. great news.
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -839,11 +839,11 @@
   </sheetPr>
   <dimension ref="A1:K307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D122" activeCellId="0" sqref="D122"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D52" activeCellId="0" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
@@ -2265,7 +2265,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
tweaked lacclair estimates, they looked wrong, and updated snow_cam_detail to match up.
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3441705-62C8-4660-BEF8-52C4F9521665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004A8D86-3703-4781-BF7A-A5629AAE7AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-324" yWindow="576" windowWidth="17280" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="312">
   <si>
     <t>Camera</t>
   </si>
@@ -958,6 +958,9 @@
   </si>
   <si>
     <t>tammela</t>
+  </si>
+  <si>
+    <t>glees_2023_05_28_101805.jpg (1296×960)</t>
   </si>
 </sst>
 </file>
@@ -1443,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B248" sqref="B248"/>
+    <sheetView tabSelected="1" topLeftCell="A427" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C434" sqref="C434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2026,7 +2029,7 @@
         <v>44306</v>
       </c>
       <c r="C21" s="7">
-        <v>0.9</v>
+        <v>0.94</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -3062,7 +3065,7 @@
         <v>43954</v>
       </c>
       <c r="C58" s="1">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -3286,7 +3289,7 @@
         <v>44318</v>
       </c>
       <c r="C66" s="1">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -3370,7 +3373,7 @@
         <v>44681</v>
       </c>
       <c r="C69" s="1">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -3565,7 +3568,7 @@
         <v>45054</v>
       </c>
       <c r="C76" s="1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -3725,7 +3728,7 @@
         <v>45408</v>
       </c>
       <c r="C82" s="1">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -4022,7 +4025,7 @@
         <v>44134</v>
       </c>
       <c r="C93" s="1">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -4184,7 +4187,7 @@
         <v>44520</v>
       </c>
       <c r="C99" s="1">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -5204,7 +5207,7 @@
         <v>43524</v>
       </c>
       <c r="C137" s="1">
-        <v>0.8</v>
+        <v>0.97</v>
       </c>
       <c r="D137">
         <v>0</v>
@@ -5232,7 +5235,7 @@
         <v>43609</v>
       </c>
       <c r="C138" s="1">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D138">
         <v>0</v>
@@ -5624,7 +5627,7 @@
         <v>44608</v>
       </c>
       <c r="C152" s="1">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -5993,7 +5996,7 @@
         <v>43490</v>
       </c>
       <c r="C167" s="1">
-        <v>0.1</v>
+        <v>0.32</v>
       </c>
       <c r="D167">
         <v>0</v>
@@ -6158,7 +6161,7 @@
         <v>43853</v>
       </c>
       <c r="C173" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="D173">
         <v>0</v>
@@ -8108,7 +8111,7 @@
         <v>43928</v>
       </c>
       <c r="C246" s="1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D246">
         <v>0</v>
@@ -9603,7 +9606,7 @@
         <v>43984</v>
       </c>
       <c r="C303" s="1">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -9863,13 +9866,13 @@
         <v>45074</v>
       </c>
       <c r="C313" s="1">
-        <v>0.9</v>
+        <v>0.96</v>
       </c>
       <c r="D313">
         <v>0</v>
       </c>
       <c r="E313" s="8" t="s">
-        <v>272</v>
+        <v>311</v>
       </c>
       <c r="F313">
         <v>-106.2394</v>
@@ -10695,7 +10698,7 @@
         <v>43573</v>
       </c>
       <c r="C345" s="1">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D345">
         <v>0</v>
@@ -10721,7 +10724,7 @@
         <v>43592</v>
       </c>
       <c r="C346" s="1">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="D346">
         <v>0</v>
@@ -11056,7 +11059,7 @@
         <v>44863</v>
       </c>
       <c r="C359" s="1">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D359">
         <v>0</v>
@@ -11414,7 +11417,7 @@
         <v>43592</v>
       </c>
       <c r="C373" s="1">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="D373">
         <v>0</v>
@@ -11575,7 +11578,7 @@
         <v>43976</v>
       </c>
       <c r="C380" s="1">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="D380">
         <v>0</v>
@@ -11598,7 +11601,7 @@
         <v>43984</v>
       </c>
       <c r="C381" s="1">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="D381">
         <v>0</v>
@@ -11759,7 +11762,7 @@
         <v>44347</v>
       </c>
       <c r="C388" s="1">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D388">
         <v>0</v>
@@ -12012,7 +12015,7 @@
         <v>43977</v>
       </c>
       <c r="C399" s="1">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="D399">
         <v>0</v>
@@ -12495,7 +12498,7 @@
         <v>43872</v>
       </c>
       <c r="C420" s="1">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
       <c r="D420">
         <v>0</v>
@@ -12518,7 +12521,7 @@
         <v>43907</v>
       </c>
       <c r="C421" s="1">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D421">
         <v>0</v>
@@ -12541,7 +12544,7 @@
         <v>43963</v>
       </c>
       <c r="C422" s="1">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="D422">
         <v>0</v>
@@ -12794,7 +12797,7 @@
         <v>44689</v>
       </c>
       <c r="C433" s="1">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="D433">
         <v>0</v>
@@ -13633,63 +13636,63 @@
     <hyperlink ref="E310" r:id="rId291" display="https://phenocam.nau.edu/data/archive/glees/2022/11/glees_2022_11_27_071806.jpg" xr:uid="{5094B975-0F33-40BE-B874-A81E254B5174}"/>
     <hyperlink ref="E311" r:id="rId292" display="https://phenocam.nau.edu/data/archive/glees/2022/12/glees_2022_12_27_141805.jpg" xr:uid="{7A4792F3-0312-4795-B04B-BCDB0951B1F4}"/>
     <hyperlink ref="E312" r:id="rId293" display="https://phenocam.nau.edu/data/archive/glees/2023/02/glees_2023_02_25_174805.jpg" xr:uid="{F779320D-FB2E-4CAC-8E7E-0B7F2E27E68B}"/>
-    <hyperlink ref="E313" r:id="rId294" display="https://phenocam.nau.edu/data/archive/glees/2023/02/glees_2023_02_25_174805.jpg" xr:uid="{91B91078-D2EB-4472-AE5F-521E35969643}"/>
-    <hyperlink ref="E314" r:id="rId295" display="https://phenocam.nau.edu/webcam/browse/glees/2023/07/27/" xr:uid="{C8E3C780-EC07-4537-B840-07B99DEED25B}"/>
-    <hyperlink ref="E315" r:id="rId296" display="https://phenocam.nau.edu/webcam/browse/glees/2023/08/" xr:uid="{0C819187-DC48-4F89-9813-0A0146E9F5FA}"/>
-    <hyperlink ref="E316" r:id="rId297" display="https://phenocam.nau.edu/webcam/browse/glees/2023/09/26/" xr:uid="{36C522E2-D700-4C4F-98F9-A0546BE2F81D}"/>
-    <hyperlink ref="E317" r:id="rId298" display="https://phenocam.nau.edu/data/archive/glees/2023/11/glees_2023_11_25_101805.jpg" xr:uid="{6D1CD72D-C030-4CC5-A7AF-549A10BD2546}"/>
-    <hyperlink ref="E318" r:id="rId299" display="https://phenocam.nau.edu/data/archive/glees/2024/02/glees_2024_02_24_062405.jpg" xr:uid="{5345F4CD-3564-450C-943B-70633598128C}"/>
-    <hyperlink ref="E319" r:id="rId300" display="https://phenocam.nau.edu/data/archive/glees/2024/09/glees_2024_09_23_105506.jpg" xr:uid="{4E919C48-7CBB-4E7D-9895-D0BB2CFB3163}"/>
-    <hyperlink ref="E320" r:id="rId301" display="https://phenocam.nau.edu/data/archive/glees/2024/11/glees_2024_11_22_142506.jpg" xr:uid="{14E42D84-99AA-4B45-A212-8EC3E01FE30B}"/>
-    <hyperlink ref="E321" r:id="rId302" display="https://phenocam.nau.edu/data/archive/queens/2019/01/queens_2019_01_30_100006.jpg" xr:uid="{360F97A1-32E3-4B32-8EF1-D0E2AFDD25AC}"/>
-    <hyperlink ref="E322" r:id="rId303" display="https://phenocam.nau.edu/webcam/browse/queens/2019/08/29/" xr:uid="{64300654-71D6-45F2-B166-4DAE35EC5864}"/>
-    <hyperlink ref="E323" r:id="rId304" display="https://phenocam.nau.edu/webcam/browse/queens/2020/06/" xr:uid="{3606B5EA-BE7D-4442-9176-5F6FCB4B4BA0}"/>
-    <hyperlink ref="E324" r:id="rId305" display="https://phenocam.nau.edu/webcam/browse/queens/2020/07/" xr:uid="{DFB63F6C-F29B-40B2-B756-FE377A238D6B}"/>
-    <hyperlink ref="E325" r:id="rId306" display="https://phenocam.nau.edu/webcam/browse/queens/2020/07/" xr:uid="{8BE3C269-7F7E-4102-8D0F-8E803322BA1D}"/>
-    <hyperlink ref="E326" r:id="rId307" display="https://phenocam.nau.edu/data/archive/queens/2021/01/queens_2021_01_26_133705.jpg" xr:uid="{581C972E-FAD5-4C40-81F6-BE5C2719AABE}"/>
-    <hyperlink ref="E327" r:id="rId308" display="https://phenocam.nau.edu/data/archive/queens/2021/04/queens_2021_04_26_183705.jpg" xr:uid="{8134EC7C-C2DF-4851-B86C-88CCB2699F60}"/>
-    <hyperlink ref="E328" r:id="rId309" display="https://phenocam.nau.edu/webcam/browse/queens/2021/07/" xr:uid="{39E80B6E-830D-420C-978D-CB24403FA304}"/>
-    <hyperlink ref="E329" r:id="rId310" display="https://phenocam.nau.edu/webcam/browse/queens/2021/09/29/" xr:uid="{A1F0B736-794E-45FB-812E-87EA6B13AFFA}"/>
-    <hyperlink ref="E330" r:id="rId311" display="https://phenocam.nau.edu/data/archive/queens/2022/01/queens_2022_01_24_073705.jpg" xr:uid="{C92BEEB3-7357-41C6-A5E6-717D317A2BDD}"/>
-    <hyperlink ref="E331" r:id="rId312" display="https://phenocam.nau.edu/webcam/browse/queens/2022/05/30/" xr:uid="{08C0B088-AF09-4EF3-905D-339DD7F7D166}"/>
-    <hyperlink ref="E332" r:id="rId313" display="https://phenocam.nau.edu/webcam/browse/queens/2022/08/" xr:uid="{CDDD0D64-5427-4AA4-BE50-DCF21C8A44AC}"/>
-    <hyperlink ref="E333" r:id="rId314" display="https://phenocam.nau.edu/webcam/browse/queens/2022/10/23/" xr:uid="{B6A785FC-7351-432F-83AF-200ABF0AEC47}"/>
-    <hyperlink ref="E334" r:id="rId315" display="https://phenocam.nau.edu/webcam/browse/queens/2023/06/" xr:uid="{0AD0347E-2ED3-4371-80DC-7EA8EAAAA724}"/>
-    <hyperlink ref="E335" r:id="rId316" display="https://phenocam.nau.edu/webcam/browse/queens/2023/07/" xr:uid="{693642E3-0B7D-415D-8F27-B39C16D5B5BB}"/>
-    <hyperlink ref="E336" r:id="rId317" display="https://phenocam.nau.edu/webcam/browse/queens/2023/09/" xr:uid="{C80C9464-DE78-4B01-BB15-E2B4899D7D89}"/>
-    <hyperlink ref="E337" r:id="rId318" display="https://phenocam.nau.edu/data/archive/queens/2024/01/queens_2024_01_20_170705.jpg" xr:uid="{A02E6DE4-2A3F-4711-BBD0-CCC283B58833}"/>
-    <hyperlink ref="E338" r:id="rId319" display="https://phenocam.nau.edu/data/archive/queens/2024/04/queens_2024_04_20_080705.jpg" xr:uid="{71732A73-A45E-43B7-BEA9-D0176B6680A4}"/>
-    <hyperlink ref="E339" r:id="rId320" display="https://phenocam.nau.edu/webcam/browse/queens/2024/07/" xr:uid="{BA4883D8-62EC-4BE3-9CB5-EE63A5099E48}"/>
-    <hyperlink ref="E340" r:id="rId321" display="https://phenocam.nau.edu/webcam/browse/queens/2024/09/" xr:uid="{D3B1FC12-0785-4C5F-B805-8724451A0B43}"/>
-    <hyperlink ref="E341" r:id="rId322" display="https://phenocam.nau.edu/webcam/browse/queens/2024/10/19/" xr:uid="{91474577-2D62-4B5F-8CD6-28E81DEBF0DA}"/>
-    <hyperlink ref="E342" r:id="rId323" display="https://phenocam.nau.edu/data/archive/canadaojp/2018/10/canadaojp_2018_10_18_162959.jpg" xr:uid="{290773FF-E96A-430B-89B5-8F0643BDC8A2}"/>
-    <hyperlink ref="E343" r:id="rId324" display="https://phenocam.nau.edu/data/archive/canadaojp/2018/11/canadaojp_2018_11_06_075959.jpg" xr:uid="{1F0819BD-00BB-48DD-A9B0-9AB4CCCC9C6D}"/>
-    <hyperlink ref="E344" r:id="rId325" display="https://phenocam.nau.edu/data/archive/canadaojp/2019/01/canadaojp_2019_01_17_112959.jpg" xr:uid="{A1B0AB39-29F1-42F2-9848-0F99E964C900}"/>
-    <hyperlink ref="E345" r:id="rId326" display="https://phenocam.nau.edu/data/archive/canadaojp/2019/04/canadaojp_2019_04_19_052959.jpg" xr:uid="{EE3E83E5-CD91-4EE6-B043-E4AD901B7E66}"/>
-    <hyperlink ref="E346" r:id="rId327" display="https://phenocam.nau.edu/data/archive/canadaojp/2019/05/canadaojp_2019_05_07_055959.jpg" xr:uid="{402003C0-325E-4DDE-B5C8-F49920BF9CD4}"/>
-    <hyperlink ref="E348" r:id="rId328" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/01/canadaojp_2020_01_15_172959.jpg" xr:uid="{BF63B7FE-8773-4E1B-AF38-10A9318138F0}"/>
-    <hyperlink ref="E349" r:id="rId329" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/02/canadaojp_2020_02_03_082959.jpg" xr:uid="{97357D13-902B-4AD9-97C0-B7172BE7D222}"/>
-    <hyperlink ref="E350" r:id="rId330" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/04/canadaojp_2020_04_15_145959.jpg" xr:uid="{1AEA1DE9-CAC3-4D50-BD68-91F6C040C124}"/>
-    <hyperlink ref="E351" r:id="rId331" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/05/canadaojp_2020_05_04_045959.jpg" xr:uid="{7FEFF69E-8EF3-47C2-97DC-E2FCDF6D1F66}"/>
-    <hyperlink ref="E352" r:id="rId332" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2020/08/" xr:uid="{7D494400-A0AC-4B0C-8B31-50CE9D455FD4}"/>
-    <hyperlink ref="E353" r:id="rId333" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/10/canadaojp_2020_10_14_073000.jpg" xr:uid="{BE6B4BF5-12D7-45AF-A709-93A34BEBD7B0}"/>
-    <hyperlink ref="E354" r:id="rId334" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/10/canadaojp_2020_10_31_172959.jpg" xr:uid="{7C0A5B0C-8750-43C5-BE13-04552E2E9AF0}"/>
-    <hyperlink ref="E355" r:id="rId335" display="https://phenocam.nau.edu/data/archive/canadaojp/2021/07/canadaojp_2021_07_13_090017.jpg" xr:uid="{012E2006-40F4-4D21-932F-372E49393B4C}"/>
-    <hyperlink ref="E356" r:id="rId336" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2021/08/" xr:uid="{7EC7461C-3AB0-47A8-B754-B4EE9C17ED39}"/>
-    <hyperlink ref="E357" r:id="rId337" display="https://phenocam.nau.edu/data/archive/canadaojp/2021/10/canadaojp_2021_10_31_080028.jpg" xr:uid="{497814D7-EF41-404C-8AAD-E4741DF8E19B}"/>
-    <hyperlink ref="E358" r:id="rId338" display="https://phenocam.nau.edu/data/archive/canadaojp/2022/05/canadaojp_2022_05_11_050011.jpg" xr:uid="{8CAA40C0-1C7A-4FF8-8BB2-E942B8CEE438}"/>
-    <hyperlink ref="E359" r:id="rId339" display="https://phenocam.nau.edu/data/archive/canadaojp/2022/10/canadaojp_2022_10_29_080013.jpg" xr:uid="{C3000DF7-BF58-4692-8626-749F7D0D773F}"/>
-    <hyperlink ref="E360" r:id="rId340" display="https://phenocam.nau.edu/data/archive/canadaojp/2023/01/canadaojp_2023_01_28_083014.jpg" xr:uid="{2969C543-FFEE-4527-97DE-746F39BB0BC2}"/>
-    <hyperlink ref="E361" r:id="rId341" display="https://phenocam.nau.edu/data/archive/canadaojp/2023/04/canadaojp_2023_04_10_090014.jpg" xr:uid="{F4B832AA-6FAD-4C6B-BA3D-DBE9AA5B24D8}"/>
-    <hyperlink ref="E362" r:id="rId342" display="https://phenocam.nau.edu/data/archive/canadaojp/2023/04/canadaojp_2023_04_28_203029.jpg" xr:uid="{D5C2A1F1-F3A0-4F54-869F-B2B6D674B001}"/>
-    <hyperlink ref="E363" r:id="rId343" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2023/07/10/" xr:uid="{2ECA9FF1-435F-44AE-A2D7-B86172E6B01A}"/>
-    <hyperlink ref="E364" r:id="rId344" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2023/07/" xr:uid="{12398967-610E-46D5-A894-2C8944AF6C68}"/>
-    <hyperlink ref="E365" r:id="rId345" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2023/10/09/" xr:uid="{E6742861-834D-45E2-9706-635FAAE98023}"/>
-    <hyperlink ref="E366" r:id="rId346" display="https://phenocam.nau.edu/data/archive/canadaojp/2023/10/canadaojp_2023_10_27_130014.jpg" xr:uid="{B60B8613-CA12-40FB-BCF3-7F93CB0F48CD}"/>
-    <hyperlink ref="E367" r:id="rId347" display="https://phenocam.nau.edu/data/archive/canadaojp/2024/01/canadaojp_2024_01_07_170018.jpg" xr:uid="{4B4F5252-CCC6-4800-8B5F-FF892D1A6027}"/>
-    <hyperlink ref="E368" r:id="rId348" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2024/01/26/" xr:uid="{E43DABBC-EB84-4E4C-B9B9-CE913621480E}"/>
-    <hyperlink ref="E369" r:id="rId349" display="https://phenocam.nau.edu/data/archive/canadaojp/2024/04/canadaojp_2024_04_07_200012.jpg" xr:uid="{AD1C1CC3-CC54-4F32-ABD9-063EF8DD5798}"/>
-    <hyperlink ref="E370" r:id="rId350" display="https://phenocam.nau.edu/data/archive/canadaojp/2024/04/canadaojp_2024_04_25_053015.jpg" xr:uid="{234FFA58-932A-4A85-BC44-C3309B72CE1C}"/>
+    <hyperlink ref="E314" r:id="rId294" display="https://phenocam.nau.edu/webcam/browse/glees/2023/07/27/" xr:uid="{C8E3C780-EC07-4537-B840-07B99DEED25B}"/>
+    <hyperlink ref="E315" r:id="rId295" display="https://phenocam.nau.edu/webcam/browse/glees/2023/08/" xr:uid="{0C819187-DC48-4F89-9813-0A0146E9F5FA}"/>
+    <hyperlink ref="E316" r:id="rId296" display="https://phenocam.nau.edu/webcam/browse/glees/2023/09/26/" xr:uid="{36C522E2-D700-4C4F-98F9-A0546BE2F81D}"/>
+    <hyperlink ref="E317" r:id="rId297" display="https://phenocam.nau.edu/data/archive/glees/2023/11/glees_2023_11_25_101805.jpg" xr:uid="{6D1CD72D-C030-4CC5-A7AF-549A10BD2546}"/>
+    <hyperlink ref="E318" r:id="rId298" display="https://phenocam.nau.edu/data/archive/glees/2024/02/glees_2024_02_24_062405.jpg" xr:uid="{5345F4CD-3564-450C-943B-70633598128C}"/>
+    <hyperlink ref="E319" r:id="rId299" display="https://phenocam.nau.edu/data/archive/glees/2024/09/glees_2024_09_23_105506.jpg" xr:uid="{4E919C48-7CBB-4E7D-9895-D0BB2CFB3163}"/>
+    <hyperlink ref="E320" r:id="rId300" display="https://phenocam.nau.edu/data/archive/glees/2024/11/glees_2024_11_22_142506.jpg" xr:uid="{14E42D84-99AA-4B45-A212-8EC3E01FE30B}"/>
+    <hyperlink ref="E321" r:id="rId301" display="https://phenocam.nau.edu/data/archive/queens/2019/01/queens_2019_01_30_100006.jpg" xr:uid="{360F97A1-32E3-4B32-8EF1-D0E2AFDD25AC}"/>
+    <hyperlink ref="E322" r:id="rId302" display="https://phenocam.nau.edu/webcam/browse/queens/2019/08/29/" xr:uid="{64300654-71D6-45F2-B166-4DAE35EC5864}"/>
+    <hyperlink ref="E323" r:id="rId303" display="https://phenocam.nau.edu/webcam/browse/queens/2020/06/" xr:uid="{3606B5EA-BE7D-4442-9176-5F6FCB4B4BA0}"/>
+    <hyperlink ref="E324" r:id="rId304" display="https://phenocam.nau.edu/webcam/browse/queens/2020/07/" xr:uid="{DFB63F6C-F29B-40B2-B756-FE377A238D6B}"/>
+    <hyperlink ref="E325" r:id="rId305" display="https://phenocam.nau.edu/webcam/browse/queens/2020/07/" xr:uid="{8BE3C269-7F7E-4102-8D0F-8E803322BA1D}"/>
+    <hyperlink ref="E326" r:id="rId306" display="https://phenocam.nau.edu/data/archive/queens/2021/01/queens_2021_01_26_133705.jpg" xr:uid="{581C972E-FAD5-4C40-81F6-BE5C2719AABE}"/>
+    <hyperlink ref="E327" r:id="rId307" display="https://phenocam.nau.edu/data/archive/queens/2021/04/queens_2021_04_26_183705.jpg" xr:uid="{8134EC7C-C2DF-4851-B86C-88CCB2699F60}"/>
+    <hyperlink ref="E328" r:id="rId308" display="https://phenocam.nau.edu/webcam/browse/queens/2021/07/" xr:uid="{39E80B6E-830D-420C-978D-CB24403FA304}"/>
+    <hyperlink ref="E329" r:id="rId309" display="https://phenocam.nau.edu/webcam/browse/queens/2021/09/29/" xr:uid="{A1F0B736-794E-45FB-812E-87EA6B13AFFA}"/>
+    <hyperlink ref="E330" r:id="rId310" display="https://phenocam.nau.edu/data/archive/queens/2022/01/queens_2022_01_24_073705.jpg" xr:uid="{C92BEEB3-7357-41C6-A5E6-717D317A2BDD}"/>
+    <hyperlink ref="E331" r:id="rId311" display="https://phenocam.nau.edu/webcam/browse/queens/2022/05/30/" xr:uid="{08C0B088-AF09-4EF3-905D-339DD7F7D166}"/>
+    <hyperlink ref="E332" r:id="rId312" display="https://phenocam.nau.edu/webcam/browse/queens/2022/08/" xr:uid="{CDDD0D64-5427-4AA4-BE50-DCF21C8A44AC}"/>
+    <hyperlink ref="E333" r:id="rId313" display="https://phenocam.nau.edu/webcam/browse/queens/2022/10/23/" xr:uid="{B6A785FC-7351-432F-83AF-200ABF0AEC47}"/>
+    <hyperlink ref="E334" r:id="rId314" display="https://phenocam.nau.edu/webcam/browse/queens/2023/06/" xr:uid="{0AD0347E-2ED3-4371-80DC-7EA8EAAAA724}"/>
+    <hyperlink ref="E335" r:id="rId315" display="https://phenocam.nau.edu/webcam/browse/queens/2023/07/" xr:uid="{693642E3-0B7D-415D-8F27-B39C16D5B5BB}"/>
+    <hyperlink ref="E336" r:id="rId316" display="https://phenocam.nau.edu/webcam/browse/queens/2023/09/" xr:uid="{C80C9464-DE78-4B01-BB15-E2B4899D7D89}"/>
+    <hyperlink ref="E337" r:id="rId317" display="https://phenocam.nau.edu/data/archive/queens/2024/01/queens_2024_01_20_170705.jpg" xr:uid="{A02E6DE4-2A3F-4711-BBD0-CCC283B58833}"/>
+    <hyperlink ref="E338" r:id="rId318" display="https://phenocam.nau.edu/data/archive/queens/2024/04/queens_2024_04_20_080705.jpg" xr:uid="{71732A73-A45E-43B7-BEA9-D0176B6680A4}"/>
+    <hyperlink ref="E339" r:id="rId319" display="https://phenocam.nau.edu/webcam/browse/queens/2024/07/" xr:uid="{BA4883D8-62EC-4BE3-9CB5-EE63A5099E48}"/>
+    <hyperlink ref="E340" r:id="rId320" display="https://phenocam.nau.edu/webcam/browse/queens/2024/09/" xr:uid="{D3B1FC12-0785-4C5F-B805-8724451A0B43}"/>
+    <hyperlink ref="E341" r:id="rId321" display="https://phenocam.nau.edu/webcam/browse/queens/2024/10/19/" xr:uid="{91474577-2D62-4B5F-8CD6-28E81DEBF0DA}"/>
+    <hyperlink ref="E342" r:id="rId322" display="https://phenocam.nau.edu/data/archive/canadaojp/2018/10/canadaojp_2018_10_18_162959.jpg" xr:uid="{290773FF-E96A-430B-89B5-8F0643BDC8A2}"/>
+    <hyperlink ref="E343" r:id="rId323" display="https://phenocam.nau.edu/data/archive/canadaojp/2018/11/canadaojp_2018_11_06_075959.jpg" xr:uid="{1F0819BD-00BB-48DD-A9B0-9AB4CCCC9C6D}"/>
+    <hyperlink ref="E344" r:id="rId324" display="https://phenocam.nau.edu/data/archive/canadaojp/2019/01/canadaojp_2019_01_17_112959.jpg" xr:uid="{A1B0AB39-29F1-42F2-9848-0F99E964C900}"/>
+    <hyperlink ref="E345" r:id="rId325" display="https://phenocam.nau.edu/data/archive/canadaojp/2019/04/canadaojp_2019_04_19_052959.jpg" xr:uid="{EE3E83E5-CD91-4EE6-B043-E4AD901B7E66}"/>
+    <hyperlink ref="E346" r:id="rId326" display="https://phenocam.nau.edu/data/archive/canadaojp/2019/05/canadaojp_2019_05_07_055959.jpg" xr:uid="{402003C0-325E-4DDE-B5C8-F49920BF9CD4}"/>
+    <hyperlink ref="E348" r:id="rId327" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/01/canadaojp_2020_01_15_172959.jpg" xr:uid="{BF63B7FE-8773-4E1B-AF38-10A9318138F0}"/>
+    <hyperlink ref="E349" r:id="rId328" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/02/canadaojp_2020_02_03_082959.jpg" xr:uid="{97357D13-902B-4AD9-97C0-B7172BE7D222}"/>
+    <hyperlink ref="E350" r:id="rId329" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/04/canadaojp_2020_04_15_145959.jpg" xr:uid="{1AEA1DE9-CAC3-4D50-BD68-91F6C040C124}"/>
+    <hyperlink ref="E351" r:id="rId330" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/05/canadaojp_2020_05_04_045959.jpg" xr:uid="{7FEFF69E-8EF3-47C2-97DC-E2FCDF6D1F66}"/>
+    <hyperlink ref="E352" r:id="rId331" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2020/08/" xr:uid="{7D494400-A0AC-4B0C-8B31-50CE9D455FD4}"/>
+    <hyperlink ref="E353" r:id="rId332" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/10/canadaojp_2020_10_14_073000.jpg" xr:uid="{BE6B4BF5-12D7-45AF-A709-93A34BEBD7B0}"/>
+    <hyperlink ref="E354" r:id="rId333" display="https://phenocam.nau.edu/data/archive/canadaojp/2020/10/canadaojp_2020_10_31_172959.jpg" xr:uid="{7C0A5B0C-8750-43C5-BE13-04552E2E9AF0}"/>
+    <hyperlink ref="E355" r:id="rId334" display="https://phenocam.nau.edu/data/archive/canadaojp/2021/07/canadaojp_2021_07_13_090017.jpg" xr:uid="{012E2006-40F4-4D21-932F-372E49393B4C}"/>
+    <hyperlink ref="E356" r:id="rId335" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2021/08/" xr:uid="{7EC7461C-3AB0-47A8-B754-B4EE9C17ED39}"/>
+    <hyperlink ref="E357" r:id="rId336" display="https://phenocam.nau.edu/data/archive/canadaojp/2021/10/canadaojp_2021_10_31_080028.jpg" xr:uid="{497814D7-EF41-404C-8AAD-E4741DF8E19B}"/>
+    <hyperlink ref="E358" r:id="rId337" display="https://phenocam.nau.edu/data/archive/canadaojp/2022/05/canadaojp_2022_05_11_050011.jpg" xr:uid="{8CAA40C0-1C7A-4FF8-8BB2-E942B8CEE438}"/>
+    <hyperlink ref="E359" r:id="rId338" display="https://phenocam.nau.edu/data/archive/canadaojp/2022/10/canadaojp_2022_10_29_080013.jpg" xr:uid="{C3000DF7-BF58-4692-8626-749F7D0D773F}"/>
+    <hyperlink ref="E360" r:id="rId339" display="https://phenocam.nau.edu/data/archive/canadaojp/2023/01/canadaojp_2023_01_28_083014.jpg" xr:uid="{2969C543-FFEE-4527-97DE-746F39BB0BC2}"/>
+    <hyperlink ref="E361" r:id="rId340" display="https://phenocam.nau.edu/data/archive/canadaojp/2023/04/canadaojp_2023_04_10_090014.jpg" xr:uid="{F4B832AA-6FAD-4C6B-BA3D-DBE9AA5B24D8}"/>
+    <hyperlink ref="E362" r:id="rId341" display="https://phenocam.nau.edu/data/archive/canadaojp/2023/04/canadaojp_2023_04_28_203029.jpg" xr:uid="{D5C2A1F1-F3A0-4F54-869F-B2B6D674B001}"/>
+    <hyperlink ref="E363" r:id="rId342" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2023/07/10/" xr:uid="{2ECA9FF1-435F-44AE-A2D7-B86172E6B01A}"/>
+    <hyperlink ref="E364" r:id="rId343" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2023/07/" xr:uid="{12398967-610E-46D5-A894-2C8944AF6C68}"/>
+    <hyperlink ref="E365" r:id="rId344" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2023/10/09/" xr:uid="{E6742861-834D-45E2-9706-635FAAE98023}"/>
+    <hyperlink ref="E366" r:id="rId345" display="https://phenocam.nau.edu/data/archive/canadaojp/2023/10/canadaojp_2023_10_27_130014.jpg" xr:uid="{B60B8613-CA12-40FB-BCF3-7F93CB0F48CD}"/>
+    <hyperlink ref="E367" r:id="rId346" display="https://phenocam.nau.edu/data/archive/canadaojp/2024/01/canadaojp_2024_01_07_170018.jpg" xr:uid="{4B4F5252-CCC6-4800-8B5F-FF892D1A6027}"/>
+    <hyperlink ref="E368" r:id="rId347" display="https://phenocam.nau.edu/webcam/browse/canadaojp/2024/01/26/" xr:uid="{E43DABBC-EB84-4E4C-B9B9-CE913621480E}"/>
+    <hyperlink ref="E369" r:id="rId348" display="https://phenocam.nau.edu/data/archive/canadaojp/2024/04/canadaojp_2024_04_07_200012.jpg" xr:uid="{AD1C1CC3-CC54-4F32-ABD9-063EF8DD5798}"/>
+    <hyperlink ref="E370" r:id="rId349" display="https://phenocam.nau.edu/data/archive/canadaojp/2024/04/canadaojp_2024_04_25_053015.jpg" xr:uid="{234FFA58-932A-4A85-BC44-C3309B72CE1C}"/>
+    <hyperlink ref="E313" r:id="rId350" display="https://phenocam.nau.edu/data/archive/glees/2023/05/glees_2023_05_28_101805.jpg" xr:uid="{9774200D-54B4-40DA-BC49-62011D659168}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId351"/>

</xml_diff>

<commit_message>
some changes in the excels
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -8,15 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004A8D86-3703-4781-BF7A-A5629AAE7AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430377A5-C3B3-4FF9-AB54-B65A44B224CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-324" yWindow="576" windowWidth="17280" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -1446,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A427" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C434" sqref="C434"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8111,7 +8120,7 @@
         <v>43928</v>
       </c>
       <c r="C246" s="1">
-        <v>0.9</v>
+        <v>0.87</v>
       </c>
       <c r="D246">
         <v>0</v>

</xml_diff>

<commit_message>
some small changes to the cam_details and timeline, related to the Landsat data gathering.
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430377A5-C3B3-4FF9-AB54-B65A44B224CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F863748A-D7B9-4F50-996A-A8C78ADE1587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2928" yWindow="2736" windowWidth="17280" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1455,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="F2:G2"/>
+    <sheetView tabSelected="1" topLeftCell="A337" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F343" sqref="F343:G343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3074,7 +3074,7 @@
         <v>43954</v>
       </c>
       <c r="C58" s="1">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="D58">
         <v>0</v>

</xml_diff>

<commit_message>
slightly improved further, and I think some of my classifications are wrong
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -1200,19 +1200,19 @@
   </sheetPr>
   <dimension ref="A1:K456"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A205" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C238" activeCellId="0" sqref="C238"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="8.89"/>
   </cols>
@@ -2819,7 +2819,7 @@
         <v>43954</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>0</v>
@@ -3043,7 +3043,7 @@
         <v>44318</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>0</v>
@@ -3482,7 +3482,7 @@
         <v>45408</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>0</v>
@@ -7627,7 +7627,7 @@
         <v>45233</v>
       </c>
       <c r="C237" s="1" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D237" s="0" t="n">
         <v>0</v>
@@ -10452,7 +10452,7 @@
         <v>43573</v>
       </c>
       <c r="C345" s="1" t="n">
-        <v>0.33</v>
+        <v>0.7</v>
       </c>
       <c r="D345" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
final FSC estimation plots for the poster.
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -1200,17 +1200,17 @@
   </sheetPr>
   <dimension ref="A1:K456"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A313" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E359" activeCellId="0" sqref="E359"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.44"/>
@@ -10452,7 +10452,7 @@
         <v>43573</v>
       </c>
       <c r="C345" s="1" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D345" s="0" t="n">
         <v>0</v>
@@ -10813,7 +10813,7 @@
         <v>44863</v>
       </c>
       <c r="C359" s="1" t="n">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D359" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
new dataframe? or maybe not I don't see any new pickles.
</commit_message>
<xml_diff>
--- a/snow_cam_details.xlsx
+++ b/snow_cam_details.xlsx
@@ -1204,19 +1204,19 @@
   </sheetPr>
   <dimension ref="A1:K456"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H102" activeCellId="0" sqref="H102:H121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A415" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D403" activeCellId="0" sqref="D403"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="8.89"/>
   </cols>
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>19</v>
@@ -2672,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>52</v>
@@ -3176,7 +3176,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>68</v>
@@ -4539,7 +4539,7 @@
         <v>1</v>
       </c>
       <c r="D126" s="0" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="E126" s="7" t="s">
         <v>81</v>
@@ -4701,7 +4701,7 @@
         <v>1</v>
       </c>
       <c r="D132" s="0" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="E132" s="7" t="s">
         <v>87</v>
@@ -7958,7 +7958,7 @@
         <v>1</v>
       </c>
       <c r="D253" s="0" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="E253" s="7" t="s">
         <v>186</v>
@@ -8662,7 +8662,7 @@
         <v>1</v>
       </c>
       <c r="D280" s="0" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="E280" s="7" t="s">
         <v>213</v>
@@ -11713,7 +11713,7 @@
         <v>1</v>
       </c>
       <c r="D402" s="0" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F402" s="0" t="n">
         <v>29.60989</v>

</xml_diff>